<commit_message>
raw score saving as csv  and keyword update and re-run
</commit_message>
<xml_diff>
--- a/data/cocurricular_competencies.xlsx
+++ b/data/cocurricular_competencies.xlsx
@@ -1,248 +1,62 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rad/Desktop/UNi/proj/EER/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD88404-3D47-414A-A5EF-2DA4FAA338E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="25160" yWindow="760" windowWidth="42000" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Modified keyword Classification" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="59">
-  <si>
-    <t>Comptency</t>
-  </si>
-  <si>
-    <t>keyword</t>
-  </si>
-  <si>
-    <t>e@UBCV</t>
-  </si>
-  <si>
-    <t>e@UBCO</t>
-  </si>
-  <si>
-    <t>UBC Social Enterprise Club</t>
-  </si>
-  <si>
-    <t>eProjects UBC</t>
-  </si>
-  <si>
-    <t>Enactus UBC</t>
-  </si>
-  <si>
-    <t>Innovation UBC Hub</t>
-  </si>
-  <si>
-    <t>Summit Leaders</t>
-  </si>
-  <si>
-    <t>UBC Sauder LIFT</t>
-  </si>
-  <si>
-    <t>UBC MBA Innovation &amp; Entrepreneurship club</t>
-  </si>
-  <si>
-    <t>Innovation on Board</t>
-  </si>
-  <si>
-    <t>Engineers without borders</t>
-  </si>
-  <si>
-    <t>Startup Pitch Competition event: UBC SOAR</t>
-  </si>
-  <si>
-    <t>Entrepreneurship and Entrepreneurial Mindset</t>
-  </si>
-  <si>
-    <t>Entrepreneur types, traits, key behaviours</t>
-  </si>
-  <si>
-    <t>Opportunity Recognition</t>
-  </si>
-  <si>
-    <t>opportunity identification, opportunity recognition, need finding, problem identification</t>
-  </si>
-  <si>
-    <t>Market Research</t>
-  </si>
-  <si>
-    <t>market research, primary research, secondary research</t>
-  </si>
-  <si>
-    <t>Product Development</t>
-  </si>
-  <si>
-    <t>product research, prototype, MVP, product, service development</t>
-  </si>
-  <si>
-    <t>Marketing</t>
-  </si>
-  <si>
-    <t>marketing, channel marketing, sales, go to market strategy</t>
-  </si>
-  <si>
-    <t>Business Modeling</t>
-  </si>
-  <si>
-    <t>business model, business model canvas, go to market plan, venture forming</t>
-  </si>
-  <si>
-    <t>Managerial Decision Making</t>
-  </si>
-  <si>
-    <t>group, project, team, management, project management, lead, decision-making</t>
-  </si>
-  <si>
-    <t>Legal Issues</t>
-  </si>
-  <si>
-    <t>legal matters, contracts, intellectual property, copyright</t>
-  </si>
-  <si>
-    <t>Financial Decision Making</t>
-  </si>
-  <si>
-    <t>financial, venture capital, financial modelling, investment/investing, revenue, funding</t>
-  </si>
-  <si>
-    <t>Observational skills</t>
-  </si>
-  <si>
-    <t>observing, questioning, seeing, sensing</t>
-  </si>
-  <si>
-    <t>Creativity skills</t>
-  </si>
-  <si>
-    <t>associating, creative thinking, innovative thinking, idea generation, prototyping, experimenting</t>
-  </si>
-  <si>
-    <t>Problem solving skills</t>
-  </si>
-  <si>
-    <t>problem solving, problem identification, opportunity identification</t>
-  </si>
-  <si>
-    <t>Communication skills</t>
-  </si>
-  <si>
-    <t>presentation, present, pitch, communication, visual thinking, sketch, map, write, design, storytelling</t>
-  </si>
-  <si>
-    <t>Decision-making skills</t>
-  </si>
-  <si>
-    <t>analytical thinking, critical thinking, assess, evaluate</t>
-  </si>
-  <si>
-    <t>Planning and project managing skills</t>
-  </si>
-  <si>
-    <t>testing, process mapping, roadmap, project manage</t>
-  </si>
-  <si>
-    <t>Networking skills</t>
-  </si>
-  <si>
-    <t>team forming, team building, networking</t>
-  </si>
-  <si>
-    <t>Negotiating skills</t>
-  </si>
-  <si>
-    <t>team management, persuasive, empathy, stakeholder engagement</t>
-  </si>
-  <si>
-    <t>Self-Aware</t>
-  </si>
-  <si>
-    <t>risk-tolerant, open, take initiative, enterprising, committed, traits</t>
-  </si>
-  <si>
-    <t>Enterprising Mindset</t>
-  </si>
-  <si>
-    <t>curiosity, self-motivated, experimental, confident, competitive, pro-active</t>
-  </si>
-  <si>
-    <t>Self-Directed</t>
-  </si>
-  <si>
-    <t>optional readings, supplemental activities, canvas discussions, goal oriented</t>
-  </si>
-  <si>
-    <t>Teamwork</t>
-  </si>
-  <si>
-    <t>networking, empathy, group management</t>
-  </si>
-  <si>
-    <t>Uncertainty Management</t>
-  </si>
-  <si>
-    <t>uncertainty, ambiguity, navigation</t>
-  </si>
-  <si>
-    <t>LaunchWeek</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="5">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF7030A0"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color rgb="FF7030A0"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="5" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="8" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="8" tint="-0.249977111117893"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
       <sz val="12"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="4">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -287,32 +101,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -335,14 +138,74 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -642,70 +505,105 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="39.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="74.1640625" bestFit="1" customWidth="1"/>
+    <col width="39.83203125" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="88.83203125" bestFit="1" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="7"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
+    <row r="1">
+      <c r="A1" s="5" t="inlineStr">
+        <is>
+          <t>Comptency</t>
+        </is>
+      </c>
+      <c r="B1" s="5" t="inlineStr">
+        <is>
+          <t>keyword</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>e@UBCV</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>e@UBCO</t>
+        </is>
+      </c>
+      <c r="E1" s="4" t="inlineStr">
+        <is>
+          <t>UBC Social Enterprise Club</t>
+        </is>
+      </c>
+      <c r="F1" s="4" t="inlineStr">
+        <is>
+          <t>eProjects UBC</t>
+        </is>
+      </c>
+      <c r="G1" s="4" t="inlineStr">
+        <is>
+          <t>Enactus UBC</t>
+        </is>
+      </c>
+      <c r="H1" s="4" t="inlineStr">
+        <is>
+          <t>Innovation UBC Hub</t>
+        </is>
+      </c>
+      <c r="I1" s="4" t="inlineStr">
+        <is>
+          <t>Summit Leaders</t>
+        </is>
+      </c>
+      <c r="J1" s="4" t="inlineStr">
+        <is>
+          <t>UBC Sauder LIFT</t>
+        </is>
+      </c>
+      <c r="K1" s="4" t="inlineStr">
+        <is>
+          <t>UBC MBA Innovation &amp; Entrepreneurship club</t>
+        </is>
+      </c>
+      <c r="L1" s="4" t="inlineStr">
+        <is>
+          <t>Innovation on Board</t>
+        </is>
+      </c>
+      <c r="M1" s="4" t="inlineStr">
+        <is>
+          <t>Engineers without borders</t>
+        </is>
+      </c>
+      <c r="N1" s="4" t="inlineStr">
+        <is>
+          <t>Startup Pitch Competition event: UBC SOAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Entrepreneurial Mindset</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>entrepreneur types, traits, openness, curiosity, growth mindset, resoucefulness, resilience, grit</t>
+        </is>
       </c>
       <c r="C2" t="b">
         <v>1</v>
@@ -732,7 +630,7 @@
         <v>1</v>
       </c>
       <c r="K2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2" t="b">
         <v>1</v>
@@ -744,12 +642,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Opportunity Recognition</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>opportunity identification, opportunity recognition, need finding, problem identification</t>
+        </is>
       </c>
       <c r="C3" t="b">
         <v>1</v>
@@ -788,12 +690,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Market Research</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>market research, primary research, secondary research, consumer research, competitor research</t>
+        </is>
       </c>
       <c r="C4" t="b">
         <v>0</v>
@@ -832,30 +738,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Product Development</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>product research, prototype, MVP, product, service development, technology research, proof of concept</t>
+        </is>
       </c>
       <c r="C5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" t="b">
         <v>0</v>
       </c>
       <c r="F5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" t="b">
         <v>0</v>
       </c>
       <c r="H5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" t="b">
         <v>0</v>
@@ -867,7 +777,7 @@
         <v>0</v>
       </c>
       <c r="L5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5" t="b">
         <v>0</v>
@@ -876,18 +786,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
-        <v>23</v>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Marketing</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>marketing, channel marketing, sales, go to market strategy, customer discovery, customer validation</t>
+        </is>
       </c>
       <c r="C6" t="b">
         <v>0</v>
       </c>
       <c r="D6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="b">
         <v>0</v>
@@ -920,12 +834,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" t="s">
-        <v>25</v>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Business Modeling</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>business model, business model canvas, go to market plan, venture forming</t>
+        </is>
       </c>
       <c r="C7" t="b">
         <v>1</v>
@@ -964,12 +882,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" t="s">
-        <v>27</v>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Managerial Decision Making</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>group, project, team, management, project management, lead, decision-making</t>
+        </is>
       </c>
       <c r="C8" t="b">
         <v>1</v>
@@ -1008,12 +930,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" t="s">
-        <v>29</v>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Legal </t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>legal matters, contracts, intellectual property, copyright, agreements, trade secrets</t>
+        </is>
       </c>
       <c r="C9" t="b">
         <v>0</v>
@@ -1052,12 +978,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" t="s">
-        <v>31</v>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Financial Decision Making</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>financial, venture capital, financial modelling, investment/investing, revenue, funding</t>
+        </is>
       </c>
       <c r="C10" t="b">
         <v>0</v>
@@ -1096,12 +1026,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" t="s">
-        <v>33</v>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>Observational skills</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>observing, questioning, seeing, sensing</t>
+        </is>
       </c>
       <c r="C11" t="b">
         <v>1</v>
@@ -1140,12 +1074,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" t="s">
-        <v>35</v>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>Creativity skills</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>associating, creative thinking, innovative thinking, idea generation, prototyping, experimenting</t>
+        </is>
       </c>
       <c r="C12" t="b">
         <v>1</v>
@@ -1184,12 +1122,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" t="s">
-        <v>37</v>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>Problem solving skills</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>problem solving, problem identification, opportunity identification</t>
+        </is>
       </c>
       <c r="C13" t="b">
         <v>0</v>
@@ -1228,12 +1170,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" t="s">
-        <v>39</v>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>Communication skills</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>presentation, present, pitch, communication, visual thinking, sketch, map, write, design, storytelling</t>
+        </is>
       </c>
       <c r="C14" t="b">
         <v>1</v>
@@ -1272,12 +1218,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" t="s">
-        <v>41</v>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>Decision-making skills</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>analytical thinking, critical thinking, assess, evaluate</t>
+        </is>
       </c>
       <c r="C15" t="b">
         <v>1</v>
@@ -1316,12 +1266,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" t="s">
-        <v>43</v>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>Planning and project managing skills</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>testing, process mapping, roadmap, project manage</t>
+        </is>
       </c>
       <c r="C16" t="b">
         <v>1</v>
@@ -1360,12 +1314,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" t="s">
-        <v>45</v>
+    <row r="17">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>Networking skills</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>team forming, team building, connections, contacts, relationships</t>
+        </is>
       </c>
       <c r="C17" t="b">
         <v>1</v>
@@ -1404,12 +1362,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" t="s">
-        <v>47</v>
+    <row r="18">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>Negotiating skills</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>team management, persuasive, empathy, stakeholder engagement</t>
+        </is>
       </c>
       <c r="C18" t="b">
         <v>1</v>
@@ -1448,12 +1410,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" t="s">
-        <v>49</v>
+    <row r="19">
+      <c r="A19" s="3" t="inlineStr">
+        <is>
+          <t>Self-Aware</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>risk-tolerant, open, take initiative, enterprising, committed, traits</t>
+        </is>
       </c>
       <c r="C19" t="b">
         <v>1</v>
@@ -1492,12 +1458,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B20" t="s">
-        <v>51</v>
+    <row r="20">
+      <c r="A20" s="3" t="inlineStr">
+        <is>
+          <t>Enterprising Mindset</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>curiosity, self-motivated, experimental, confident, competitive, pro-active</t>
+        </is>
       </c>
       <c r="C20" t="b">
         <v>1</v>
@@ -1536,21 +1506,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B21" t="s">
-        <v>53</v>
+    <row r="21">
+      <c r="A21" s="3" t="inlineStr">
+        <is>
+          <t>Self-Directed</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>readings, supplemental activities, goal oriented, take initiative, independent, self-starter</t>
+        </is>
       </c>
       <c r="C21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" t="b">
         <v>1</v>
@@ -1562,10 +1536,10 @@
         <v>0</v>
       </c>
       <c r="I21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K21" t="b">
         <v>0</v>
@@ -1580,12 +1554,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22" t="s">
-        <v>55</v>
+    <row r="22">
+      <c r="A22" s="3" t="inlineStr">
+        <is>
+          <t>Teamwork</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>networking, empathy, group management, co-founders, peers, colleagues, partners</t>
+        </is>
       </c>
       <c r="C22" t="b">
         <v>1</v>
@@ -1612,10 +1590,10 @@
         <v>1</v>
       </c>
       <c r="K22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M22" t="b">
         <v>1</v>
@@ -1624,42 +1602,46 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B23" t="s">
-        <v>57</v>
+    <row r="23">
+      <c r="A23" s="3" t="inlineStr">
+        <is>
+          <t>Uncertainty Management</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>uncertainty, ambiguity, navigation, unfamiliar, volitility, risk, complexity</t>
+        </is>
       </c>
       <c r="C23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23" t="b">
         <v>0</v>
       </c>
       <c r="I23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M23" t="b">
         <v>0</v>
@@ -1670,165 +1652,231 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:N1048576">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="false">
+    <cfRule type="containsText" priority="2" operator="containsText" dxfId="1" text="false">
       <formula>NOT(ISERROR(SEARCH("false",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="true">
+    <cfRule type="containsText" priority="1" operator="containsText" dxfId="0" text="true">
       <formula>NOT(ISERROR(SEARCH("true",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C1" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D1" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C1" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D1" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="A1" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>58</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>e@UBCV</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>e@UBCO</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>UBC Social Enterprise Club</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>eProjects UBC</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Enactus UBC</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Innovation UBC Hub</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Summit Leaders</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>UBC Sauder LIFT</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>UBC MBA Innovation &amp; Entrepreneurship club</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Innovation on Board</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Engineers without borders</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Startup Pitch Competition event: UBC SOAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>LaunchWeek</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A1" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:N23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
+    <row r="1">
+      <c r="A1" s="6" t="inlineStr">
+        <is>
+          <t>Comptency</t>
+        </is>
+      </c>
+      <c r="B1" s="6" t="inlineStr">
+        <is>
+          <t>keyword</t>
+        </is>
+      </c>
+      <c r="C1" s="6" t="inlineStr">
+        <is>
+          <t>e@UBCV</t>
+        </is>
+      </c>
+      <c r="D1" s="6" t="inlineStr">
+        <is>
+          <t>e@UBCO</t>
+        </is>
+      </c>
+      <c r="E1" s="6" t="inlineStr">
+        <is>
+          <t>UBC Social Enterprise Club</t>
+        </is>
+      </c>
+      <c r="F1" s="6" t="inlineStr">
+        <is>
+          <t>eProjects UBC</t>
+        </is>
+      </c>
+      <c r="G1" s="6" t="inlineStr">
+        <is>
+          <t>Enactus UBC</t>
+        </is>
+      </c>
+      <c r="H1" s="6" t="inlineStr">
+        <is>
+          <t>Innovation UBC Hub</t>
+        </is>
+      </c>
+      <c r="I1" s="6" t="inlineStr">
+        <is>
+          <t>Summit Leaders</t>
+        </is>
+      </c>
+      <c r="J1" s="6" t="inlineStr">
+        <is>
+          <t>UBC Sauder LIFT</t>
+        </is>
+      </c>
+      <c r="K1" s="6" t="inlineStr">
+        <is>
+          <t>UBC MBA Innovation &amp; Entrepreneurship club</t>
+        </is>
+      </c>
+      <c r="L1" s="6" t="inlineStr">
+        <is>
+          <t>Innovation on Board</t>
+        </is>
+      </c>
+      <c r="M1" s="6" t="inlineStr">
+        <is>
+          <t>Engineers without borders</t>
+        </is>
+      </c>
+      <c r="N1" s="6" t="inlineStr">
+        <is>
+          <t>Startup Pitch Competition event: UBC SOAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Entrepreneurial Mindset</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>entrepreneur types, traits, openness, curiosity, growth mindset, resoucefulness, resilience, grit</t>
+        </is>
       </c>
       <c r="C2" t="b">
         <v>1</v>
@@ -1855,7 +1903,7 @@
         <v>1</v>
       </c>
       <c r="K2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2" t="b">
         <v>1</v>
@@ -1867,12 +1915,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Opportunity Recognition</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>opportunity identification, opportunity recognition, need finding, problem identification</t>
+        </is>
       </c>
       <c r="C3" t="b">
         <v>1</v>
@@ -1911,12 +1963,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Market Research</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>market research, primary research, secondary research, consumer research, competitor research</t>
+        </is>
       </c>
       <c r="C4" t="b">
         <v>0</v>
@@ -1955,30 +2011,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Product Development</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>product research, prototype, MVP, product, service development, technology research, proof of concept</t>
+        </is>
       </c>
       <c r="C5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" t="b">
         <v>0</v>
       </c>
       <c r="F5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" t="b">
         <v>0</v>
       </c>
       <c r="H5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" t="b">
         <v>0</v>
@@ -1990,7 +2050,7 @@
         <v>0</v>
       </c>
       <c r="L5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5" t="b">
         <v>0</v>
@@ -1999,18 +2059,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
-        <v>23</v>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Marketing</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>marketing, channel marketing, sales, go to market strategy, customer discovery, customer validation</t>
+        </is>
       </c>
       <c r="C6" t="b">
         <v>0</v>
       </c>
       <c r="D6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="b">
         <v>0</v>
@@ -2043,12 +2107,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" t="s">
-        <v>25</v>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Business Modeling</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>business model, business model canvas, go to market plan, venture forming</t>
+        </is>
       </c>
       <c r="C7" t="b">
         <v>1</v>
@@ -2087,12 +2155,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" t="s">
-        <v>27</v>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Managerial Decision Making</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>group, project, team, management, project management, lead, decision-making</t>
+        </is>
       </c>
       <c r="C8" t="b">
         <v>1</v>
@@ -2131,12 +2203,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" t="s">
-        <v>29</v>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Legal </t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>legal matters, contracts, intellectual property, copyright, agreements, trade secrets</t>
+        </is>
       </c>
       <c r="C9" t="b">
         <v>0</v>
@@ -2175,12 +2251,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" t="s">
-        <v>31</v>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Financial Decision Making</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>financial, venture capital, financial modelling, investment/investing, revenue, funding</t>
+        </is>
       </c>
       <c r="C10" t="b">
         <v>0</v>
@@ -2219,12 +2299,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" t="s">
-        <v>33</v>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Observational skills</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>observing, questioning, seeing, sensing</t>
+        </is>
       </c>
       <c r="C11" t="b">
         <v>1</v>
@@ -2263,12 +2347,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" t="s">
-        <v>35</v>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Creativity skills</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>associating, creative thinking, innovative thinking, idea generation, prototyping, experimenting</t>
+        </is>
       </c>
       <c r="C12" t="b">
         <v>1</v>
@@ -2307,12 +2395,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" t="s">
-        <v>37</v>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Problem solving skills</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>problem solving, problem identification, opportunity identification</t>
+        </is>
       </c>
       <c r="C13" t="b">
         <v>0</v>
@@ -2351,12 +2443,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" t="s">
-        <v>39</v>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Communication skills</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>presentation, present, pitch, communication, visual thinking, sketch, map, write, design, storytelling</t>
+        </is>
       </c>
       <c r="C14" t="b">
         <v>1</v>
@@ -2395,12 +2491,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" t="s">
-        <v>41</v>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Decision-making skills</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>analytical thinking, critical thinking, assess, evaluate</t>
+        </is>
       </c>
       <c r="C15" t="b">
         <v>1</v>
@@ -2439,12 +2539,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" t="s">
-        <v>43</v>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Planning and project managing skills</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>testing, process mapping, roadmap, project manage</t>
+        </is>
       </c>
       <c r="C16" t="b">
         <v>1</v>
@@ -2483,12 +2587,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" t="s">
-        <v>45</v>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Networking skills</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>team forming, team building, connections, contacts, relationships</t>
+        </is>
       </c>
       <c r="C17" t="b">
         <v>1</v>
@@ -2527,12 +2635,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" t="s">
-        <v>47</v>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Negotiating skills</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>team management, persuasive, empathy, stakeholder engagement</t>
+        </is>
       </c>
       <c r="C18" t="b">
         <v>1</v>
@@ -2571,12 +2683,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" t="s">
-        <v>49</v>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Self-Aware</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>risk-tolerant, open, take initiative, enterprising, committed, traits</t>
+        </is>
       </c>
       <c r="C19" t="b">
         <v>1</v>
@@ -2615,12 +2731,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>50</v>
-      </c>
-      <c r="B20" t="s">
-        <v>51</v>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Enterprising Mindset</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>curiosity, self-motivated, experimental, confident, competitive, pro-active</t>
+        </is>
       </c>
       <c r="C20" t="b">
         <v>1</v>
@@ -2659,21 +2779,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>52</v>
-      </c>
-      <c r="B21" t="s">
-        <v>53</v>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Self-Directed</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>readings, supplemental activities, goal oriented, take initiative, independent, self-starter</t>
+        </is>
       </c>
       <c r="C21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" t="b">
         <v>1</v>
@@ -2685,10 +2809,10 @@
         <v>0</v>
       </c>
       <c r="I21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K21" t="b">
         <v>0</v>
@@ -2703,12 +2827,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22" t="s">
-        <v>55</v>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Teamwork</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>networking, empathy, group management, co-founders, peers, colleagues, partners</t>
+        </is>
       </c>
       <c r="C22" t="b">
         <v>1</v>
@@ -2735,10 +2863,10 @@
         <v>1</v>
       </c>
       <c r="K22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M22" t="b">
         <v>1</v>
@@ -2747,42 +2875,46 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>56</v>
-      </c>
-      <c r="B23" t="s">
-        <v>57</v>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Uncertainty Management</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>uncertainty, ambiguity, navigation, unfamiliar, volitility, risk, complexity</t>
+        </is>
       </c>
       <c r="C23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23" t="b">
         <v>0</v>
       </c>
       <c r="I23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M23" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
add the syllabi data excel sheet
</commit_message>
<xml_diff>
--- a/data/cocurricular_competencies.xlsx
+++ b/data/cocurricular_competencies.xlsx
@@ -1,62 +1,261 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rad/Desktop/UNi/proj/EER/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEDA9F14-20A3-CB4D-BC5B-1E7DE262A3DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Modified keyword Classification" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Modified keyword Classification" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="63">
+  <si>
+    <t>Comptency</t>
+  </si>
+  <si>
+    <t>keyword</t>
+  </si>
+  <si>
+    <t>e@UBCV</t>
+  </si>
+  <si>
+    <t>e@UBCO</t>
+  </si>
+  <si>
+    <t>UBC Social Enterprise Club</t>
+  </si>
+  <si>
+    <t>eProjects UBC</t>
+  </si>
+  <si>
+    <t>Enactus UBC</t>
+  </si>
+  <si>
+    <t>Innovation UBC Hub</t>
+  </si>
+  <si>
+    <t>Summit Leaders</t>
+  </si>
+  <si>
+    <t>UBC Sauder LIFT</t>
+  </si>
+  <si>
+    <t>UBC MBA Innovation &amp; Entrepreneurship club</t>
+  </si>
+  <si>
+    <t>Innovation on Board</t>
+  </si>
+  <si>
+    <t>Engineers without borders</t>
+  </si>
+  <si>
+    <t>Startup Pitch Competition event: UBC SOAR</t>
+  </si>
+  <si>
+    <t>Entrepreneurial Mindset</t>
+  </si>
+  <si>
+    <t>entrepreneur types, traits, openness, curiosity, growth mindset, resoucefulness, resilience, grit</t>
+  </si>
+  <si>
+    <t>Opportunity Recognition</t>
+  </si>
+  <si>
+    <t>opportunity identification, opportunity recognition, need finding, problem identification</t>
+  </si>
+  <si>
+    <t>Market Research</t>
+  </si>
+  <si>
+    <t>market research, primary research, secondary research, consumer research, competitor research, customer discovery, customer validation</t>
+  </si>
+  <si>
+    <t>Product Development</t>
+  </si>
+  <si>
+    <t>product research, prototype, MVP, product, service development, technology research, proof of concept</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>marketing, channel marketing, sales, go to market strategy</t>
+  </si>
+  <si>
+    <t>Business Modeling</t>
+  </si>
+  <si>
+    <t>business model, business model canvas, go to market plan, venture forming</t>
+  </si>
+  <si>
+    <t>Managerial Decision Making</t>
+  </si>
+  <si>
+    <t>group, project, team, management, project management, lead, decision-making</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Legal </t>
+  </si>
+  <si>
+    <t>legal matters, contracts, intellectual property, copyright, agreements, trade secrets, patents, license</t>
+  </si>
+  <si>
+    <t>Financial Decision Making</t>
+  </si>
+  <si>
+    <t>financial, venture capital, financial modelling, investment/investing, revenue, funding</t>
+  </si>
+  <si>
+    <t>Observational skills</t>
+  </si>
+  <si>
+    <t>observing, questioning, seeing, sensing</t>
+  </si>
+  <si>
+    <t>Creativity skills</t>
+  </si>
+  <si>
+    <t>associating, creative thinking, innovative thinking, idea generation, prototyping, experimenting</t>
+  </si>
+  <si>
+    <t>Problem solving skills</t>
+  </si>
+  <si>
+    <t>problem solving, problem identification, opportunity identification</t>
+  </si>
+  <si>
+    <t>Communication skills</t>
+  </si>
+  <si>
+    <t>presentation, present, pitch, communication, visual thinking, sketch, map, write, design, storytelling</t>
+  </si>
+  <si>
+    <t>Decision-making skills</t>
+  </si>
+  <si>
+    <t>analytical thinking, critical thinking, assess, evaluate</t>
+  </si>
+  <si>
+    <t>Planning and project managing skills</t>
+  </si>
+  <si>
+    <t>testing, process mapping, roadmap, project manage</t>
+  </si>
+  <si>
+    <t>Networking skills</t>
+  </si>
+  <si>
+    <t>team forming, team building, connections, contacts, relationships</t>
+  </si>
+  <si>
+    <t>Negotiating skills</t>
+  </si>
+  <si>
+    <t>team management, persuasive, empathy, stakeholder engagement</t>
+  </si>
+  <si>
+    <t>Self-Aware</t>
+  </si>
+  <si>
+    <t>risk-tolerant, open, take initiative, enterprising, committed, traits</t>
+  </si>
+  <si>
+    <t>Enterprising Mindset</t>
+  </si>
+  <si>
+    <t>curiosity, self-motivated, experimental, confident, competitive, pro-active</t>
+  </si>
+  <si>
+    <t>Self-Directed</t>
+  </si>
+  <si>
+    <t>readings, supplemental activities, goal oriented, take initiative, independent, self-starter</t>
+  </si>
+  <si>
+    <t>Teamwork</t>
+  </si>
+  <si>
+    <t>networking, empathy, group management, co-founders, peers, colleagues, partners</t>
+  </si>
+  <si>
+    <t>Uncertainty Management</t>
+  </si>
+  <si>
+    <t>uncertainty, ambiguity, navigation, unfamiliar, volitility, risk, complexity</t>
+  </si>
+  <si>
+    <t>LaunchWeek</t>
+  </si>
+  <si>
+    <t>market research, primary research, secondary research, consumer research, competitor research</t>
+  </si>
+  <si>
+    <t>marketing, channel marketing, sales, go to market strategy, customer discovery, customer validation</t>
+  </si>
+  <si>
+    <t>legal matters, contracts, intellectual property, copyright, agreements, trade secrets</t>
+  </si>
+  <si>
+    <t>Enterprising Traits</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color rgb="FF7030A0"/>
+    </font>
+    <font>
       <sz val="12"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="4" tint="0.39997558519241921"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="5" tint="-0.249977111117893"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="4" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="8" tint="-0.249977111117893"/>
-      <sz val="12"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="1"/>
-      <sz val="12"/>
     </font>
   </fonts>
   <fills count="4">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -102,15 +301,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -138,74 +337,14 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -505,105 +644,69 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col width="39.83203125" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="88.83203125" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col min="1" max="1" width="39.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="117.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="5" t="inlineStr">
-        <is>
-          <t>Comptency</t>
-        </is>
-      </c>
-      <c r="B1" s="5" t="inlineStr">
-        <is>
-          <t>keyword</t>
-        </is>
-      </c>
-      <c r="C1" s="4" t="inlineStr">
-        <is>
-          <t>e@UBCV</t>
-        </is>
-      </c>
-      <c r="D1" s="4" t="inlineStr">
-        <is>
-          <t>e@UBCO</t>
-        </is>
-      </c>
-      <c r="E1" s="4" t="inlineStr">
-        <is>
-          <t>UBC Social Enterprise Club</t>
-        </is>
-      </c>
-      <c r="F1" s="4" t="inlineStr">
-        <is>
-          <t>eProjects UBC</t>
-        </is>
-      </c>
-      <c r="G1" s="4" t="inlineStr">
-        <is>
-          <t>Enactus UBC</t>
-        </is>
-      </c>
-      <c r="H1" s="4" t="inlineStr">
-        <is>
-          <t>Innovation UBC Hub</t>
-        </is>
-      </c>
-      <c r="I1" s="4" t="inlineStr">
-        <is>
-          <t>Summit Leaders</t>
-        </is>
-      </c>
-      <c r="J1" s="4" t="inlineStr">
-        <is>
-          <t>UBC Sauder LIFT</t>
-        </is>
-      </c>
-      <c r="K1" s="4" t="inlineStr">
-        <is>
-          <t>UBC MBA Innovation &amp; Entrepreneurship club</t>
-        </is>
-      </c>
-      <c r="L1" s="4" t="inlineStr">
-        <is>
-          <t>Innovation on Board</t>
-        </is>
-      </c>
-      <c r="M1" s="4" t="inlineStr">
-        <is>
-          <t>Engineers without borders</t>
-        </is>
-      </c>
-      <c r="N1" s="4" t="inlineStr">
-        <is>
-          <t>Startup Pitch Competition event: UBC SOAR</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>Entrepreneurial Mindset</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>entrepreneur types, traits, openness, curiosity, growth mindset, resoucefulness, resilience, grit</t>
-        </is>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
@@ -642,16 +745,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Opportunity Recognition</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>opportunity identification, opportunity recognition, need finding, problem identification</t>
-        </is>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
       </c>
       <c r="C3" t="b">
         <v>1</v>
@@ -690,16 +789,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>Market Research</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>market research, primary research, secondary research, consumer research, competitor research</t>
-        </is>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
@@ -738,16 +833,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>Product Development</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>product research, prototype, MVP, product, service development, technology research, proof of concept</t>
-        </is>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
       </c>
       <c r="C5" t="b">
         <v>1</v>
@@ -786,16 +877,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>Marketing</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>marketing, channel marketing, sales, go to market strategy, customer discovery, customer validation</t>
-        </is>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
       </c>
       <c r="C6" t="b">
         <v>0</v>
@@ -834,16 +921,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>Business Modeling</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>business model, business model canvas, go to market plan, venture forming</t>
-        </is>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
       </c>
       <c r="C7" t="b">
         <v>1</v>
@@ -882,16 +965,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>Managerial Decision Making</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>group, project, team, management, project management, lead, decision-making</t>
-        </is>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
       </c>
       <c r="C8" t="b">
         <v>1</v>
@@ -930,16 +1009,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Legal </t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>legal matters, contracts, intellectual property, copyright, agreements, trade secrets</t>
-        </is>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
       </c>
       <c r="C9" t="b">
         <v>0</v>
@@ -978,16 +1053,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>Financial Decision Making</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>financial, venture capital, financial modelling, investment/investing, revenue, funding</t>
-        </is>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
       </c>
       <c r="C10" t="b">
         <v>0</v>
@@ -1026,16 +1097,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="2" t="inlineStr">
-        <is>
-          <t>Observational skills</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>observing, questioning, seeing, sensing</t>
-        </is>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
       </c>
       <c r="C11" t="b">
         <v>1</v>
@@ -1074,16 +1141,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="2" t="inlineStr">
-        <is>
-          <t>Creativity skills</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>associating, creative thinking, innovative thinking, idea generation, prototyping, experimenting</t>
-        </is>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
       </c>
       <c r="C12" t="b">
         <v>1</v>
@@ -1122,16 +1185,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="2" t="inlineStr">
-        <is>
-          <t>Problem solving skills</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>problem solving, problem identification, opportunity identification</t>
-        </is>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
       </c>
       <c r="C13" t="b">
         <v>0</v>
@@ -1170,16 +1229,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="2" t="inlineStr">
-        <is>
-          <t>Communication skills</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>presentation, present, pitch, communication, visual thinking, sketch, map, write, design, storytelling</t>
-        </is>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
       </c>
       <c r="C14" t="b">
         <v>1</v>
@@ -1218,16 +1273,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="2" t="inlineStr">
-        <is>
-          <t>Decision-making skills</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>analytical thinking, critical thinking, assess, evaluate</t>
-        </is>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
       </c>
       <c r="C15" t="b">
         <v>1</v>
@@ -1266,16 +1317,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="2" t="inlineStr">
-        <is>
-          <t>Planning and project managing skills</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>testing, process mapping, roadmap, project manage</t>
-        </is>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
       </c>
       <c r="C16" t="b">
         <v>1</v>
@@ -1314,16 +1361,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="2" t="inlineStr">
-        <is>
-          <t>Networking skills</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>team forming, team building, connections, contacts, relationships</t>
-        </is>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" t="s">
+        <v>45</v>
       </c>
       <c r="C17" t="b">
         <v>1</v>
@@ -1362,16 +1405,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="2" t="inlineStr">
-        <is>
-          <t>Negotiating skills</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>team management, persuasive, empathy, stakeholder engagement</t>
-        </is>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" t="s">
+        <v>47</v>
       </c>
       <c r="C18" t="b">
         <v>1</v>
@@ -1410,16 +1449,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="3" t="inlineStr">
-        <is>
-          <t>Self-Aware</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>risk-tolerant, open, take initiative, enterprising, committed, traits</t>
-        </is>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" t="s">
+        <v>49</v>
       </c>
       <c r="C19" t="b">
         <v>1</v>
@@ -1458,16 +1493,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="3" t="inlineStr">
-        <is>
-          <t>Enterprising Mindset</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>curiosity, self-motivated, experimental, confident, competitive, pro-active</t>
-        </is>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" t="s">
+        <v>51</v>
       </c>
       <c r="C20" t="b">
         <v>1</v>
@@ -1506,16 +1537,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="3" t="inlineStr">
-        <is>
-          <t>Self-Directed</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>readings, supplemental activities, goal oriented, take initiative, independent, self-starter</t>
-        </is>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" t="s">
+        <v>53</v>
       </c>
       <c r="C21" t="b">
         <v>1</v>
@@ -1554,16 +1581,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="3" t="inlineStr">
-        <is>
-          <t>Teamwork</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>networking, empathy, group management, co-founders, peers, colleagues, partners</t>
-        </is>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" t="s">
+        <v>55</v>
       </c>
       <c r="C22" t="b">
         <v>1</v>
@@ -1602,16 +1625,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="3" t="inlineStr">
-        <is>
-          <t>Uncertainty Management</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>uncertainty, ambiguity, navigation, unfamiliar, volitility, risk, complexity</t>
-        </is>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" t="s">
+        <v>57</v>
       </c>
       <c r="C23" t="b">
         <v>1</v>
@@ -1652,231 +1671,165 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:N1048576">
-    <cfRule type="containsText" priority="2" operator="containsText" dxfId="1" text="false">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="false">
       <formula>NOT(ISERROR(SEARCH("false",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" priority="1" operator="containsText" dxfId="0" text="true">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="true">
       <formula>NOT(ISERROR(SEARCH("true",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C1" r:id="rId1"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D1" r:id="rId2"/>
+    <hyperlink ref="C1" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D1" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:A1048576"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>e@UBCV</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>e@UBCO</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>UBC Social Enterprise Club</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>eProjects UBC</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Enactus UBC</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Innovation UBC Hub</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Summit Leaders</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>UBC Sauder LIFT</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>UBC MBA Innovation &amp; Entrepreneurship club</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Innovation on Board</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Engineers without borders</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Startup Pitch Competition event: UBC SOAR</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>LaunchWeek</t>
-        </is>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A1" r:id="rId1"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A2" r:id="rId2"/>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:N23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="6" t="inlineStr">
-        <is>
-          <t>Comptency</t>
-        </is>
-      </c>
-      <c r="B1" s="6" t="inlineStr">
-        <is>
-          <t>keyword</t>
-        </is>
-      </c>
-      <c r="C1" s="6" t="inlineStr">
-        <is>
-          <t>e@UBCV</t>
-        </is>
-      </c>
-      <c r="D1" s="6" t="inlineStr">
-        <is>
-          <t>e@UBCO</t>
-        </is>
-      </c>
-      <c r="E1" s="6" t="inlineStr">
-        <is>
-          <t>UBC Social Enterprise Club</t>
-        </is>
-      </c>
-      <c r="F1" s="6" t="inlineStr">
-        <is>
-          <t>eProjects UBC</t>
-        </is>
-      </c>
-      <c r="G1" s="6" t="inlineStr">
-        <is>
-          <t>Enactus UBC</t>
-        </is>
-      </c>
-      <c r="H1" s="6" t="inlineStr">
-        <is>
-          <t>Innovation UBC Hub</t>
-        </is>
-      </c>
-      <c r="I1" s="6" t="inlineStr">
-        <is>
-          <t>Summit Leaders</t>
-        </is>
-      </c>
-      <c r="J1" s="6" t="inlineStr">
-        <is>
-          <t>UBC Sauder LIFT</t>
-        </is>
-      </c>
-      <c r="K1" s="6" t="inlineStr">
-        <is>
-          <t>UBC MBA Innovation &amp; Entrepreneurship club</t>
-        </is>
-      </c>
-      <c r="L1" s="6" t="inlineStr">
-        <is>
-          <t>Innovation on Board</t>
-        </is>
-      </c>
-      <c r="M1" s="6" t="inlineStr">
-        <is>
-          <t>Engineers without borders</t>
-        </is>
-      </c>
-      <c r="N1" s="6" t="inlineStr">
-        <is>
-          <t>Startup Pitch Competition event: UBC SOAR</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Entrepreneurial Mindset</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>entrepreneur types, traits, openness, curiosity, growth mindset, resoucefulness, resilience, grit</t>
-        </is>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
@@ -1915,16 +1868,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Opportunity Recognition</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>opportunity identification, opportunity recognition, need finding, problem identification</t>
-        </is>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
       </c>
       <c r="C3" t="b">
         <v>1</v>
@@ -1963,16 +1912,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Market Research</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>market research, primary research, secondary research, consumer research, competitor research</t>
-        </is>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>59</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
@@ -2011,16 +1956,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Product Development</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>product research, prototype, MVP, product, service development, technology research, proof of concept</t>
-        </is>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
       </c>
       <c r="C5" t="b">
         <v>1</v>
@@ -2059,16 +2000,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Marketing</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>marketing, channel marketing, sales, go to market strategy, customer discovery, customer validation</t>
-        </is>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>60</v>
       </c>
       <c r="C6" t="b">
         <v>0</v>
@@ -2107,16 +2044,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Business Modeling</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>business model, business model canvas, go to market plan, venture forming</t>
-        </is>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
       </c>
       <c r="C7" t="b">
         <v>1</v>
@@ -2155,16 +2088,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Managerial Decision Making</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>group, project, team, management, project management, lead, decision-making</t>
-        </is>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
       </c>
       <c r="C8" t="b">
         <v>1</v>
@@ -2203,16 +2132,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Legal </t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>legal matters, contracts, intellectual property, copyright, agreements, trade secrets</t>
-        </is>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>61</v>
       </c>
       <c r="C9" t="b">
         <v>0</v>
@@ -2251,16 +2176,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Financial Decision Making</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>financial, venture capital, financial modelling, investment/investing, revenue, funding</t>
-        </is>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
       </c>
       <c r="C10" t="b">
         <v>0</v>
@@ -2299,16 +2220,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Observational skills</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>observing, questioning, seeing, sensing</t>
-        </is>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
       </c>
       <c r="C11" t="b">
         <v>1</v>
@@ -2347,16 +2264,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Creativity skills</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>associating, creative thinking, innovative thinking, idea generation, prototyping, experimenting</t>
-        </is>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
       </c>
       <c r="C12" t="b">
         <v>1</v>
@@ -2395,16 +2308,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Problem solving skills</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>problem solving, problem identification, opportunity identification</t>
-        </is>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
       </c>
       <c r="C13" t="b">
         <v>0</v>
@@ -2443,16 +2352,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Communication skills</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>presentation, present, pitch, communication, visual thinking, sketch, map, write, design, storytelling</t>
-        </is>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
       </c>
       <c r="C14" t="b">
         <v>1</v>
@@ -2491,16 +2396,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Decision-making skills</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>analytical thinking, critical thinking, assess, evaluate</t>
-        </is>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
       </c>
       <c r="C15" t="b">
         <v>1</v>
@@ -2539,16 +2440,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Planning and project managing skills</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>testing, process mapping, roadmap, project manage</t>
-        </is>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
       </c>
       <c r="C16" t="b">
         <v>1</v>
@@ -2587,16 +2484,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Networking skills</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>team forming, team building, connections, contacts, relationships</t>
-        </is>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" t="s">
+        <v>45</v>
       </c>
       <c r="C17" t="b">
         <v>1</v>
@@ -2635,16 +2528,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Negotiating skills</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>team management, persuasive, empathy, stakeholder engagement</t>
-        </is>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" t="s">
+        <v>47</v>
       </c>
       <c r="C18" t="b">
         <v>1</v>
@@ -2683,16 +2572,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Self-Aware</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>risk-tolerant, open, take initiative, enterprising, committed, traits</t>
-        </is>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" t="s">
+        <v>49</v>
       </c>
       <c r="C19" t="b">
         <v>1</v>
@@ -2731,16 +2616,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Enterprising Mindset</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>curiosity, self-motivated, experimental, confident, competitive, pro-active</t>
-        </is>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" t="s">
+        <v>51</v>
       </c>
       <c r="C20" t="b">
         <v>1</v>
@@ -2779,16 +2660,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Self-Directed</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>readings, supplemental activities, goal oriented, take initiative, independent, self-starter</t>
-        </is>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" t="s">
+        <v>53</v>
       </c>
       <c r="C21" t="b">
         <v>1</v>
@@ -2827,16 +2704,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Teamwork</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>networking, empathy, group management, co-founders, peers, colleagues, partners</t>
-        </is>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" t="s">
+        <v>55</v>
       </c>
       <c r="C22" t="b">
         <v>1</v>
@@ -2875,16 +2748,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Uncertainty Management</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>uncertainty, ambiguity, navigation, unfamiliar, volitility, risk, complexity</t>
-        </is>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" t="s">
+        <v>57</v>
       </c>
       <c r="C23" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
rerun the nlp_label.py file to ensure running on new device
</commit_message>
<xml_diff>
--- a/data/cocurricular_competencies.xlsx
+++ b/data/cocurricular_competencies.xlsx
@@ -1,261 +1,62 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rad/Desktop/UNi/proj/EER/data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEDA9F14-20A3-CB4D-BC5B-1E7DE262A3DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Modified keyword Classification" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Modified keyword Classification" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="63">
-  <si>
-    <t>Comptency</t>
-  </si>
-  <si>
-    <t>keyword</t>
-  </si>
-  <si>
-    <t>e@UBCV</t>
-  </si>
-  <si>
-    <t>e@UBCO</t>
-  </si>
-  <si>
-    <t>UBC Social Enterprise Club</t>
-  </si>
-  <si>
-    <t>eProjects UBC</t>
-  </si>
-  <si>
-    <t>Enactus UBC</t>
-  </si>
-  <si>
-    <t>Innovation UBC Hub</t>
-  </si>
-  <si>
-    <t>Summit Leaders</t>
-  </si>
-  <si>
-    <t>UBC Sauder LIFT</t>
-  </si>
-  <si>
-    <t>UBC MBA Innovation &amp; Entrepreneurship club</t>
-  </si>
-  <si>
-    <t>Innovation on Board</t>
-  </si>
-  <si>
-    <t>Engineers without borders</t>
-  </si>
-  <si>
-    <t>Startup Pitch Competition event: UBC SOAR</t>
-  </si>
-  <si>
-    <t>Entrepreneurial Mindset</t>
-  </si>
-  <si>
-    <t>entrepreneur types, traits, openness, curiosity, growth mindset, resoucefulness, resilience, grit</t>
-  </si>
-  <si>
-    <t>Opportunity Recognition</t>
-  </si>
-  <si>
-    <t>opportunity identification, opportunity recognition, need finding, problem identification</t>
-  </si>
-  <si>
-    <t>Market Research</t>
-  </si>
-  <si>
-    <t>market research, primary research, secondary research, consumer research, competitor research, customer discovery, customer validation</t>
-  </si>
-  <si>
-    <t>Product Development</t>
-  </si>
-  <si>
-    <t>product research, prototype, MVP, product, service development, technology research, proof of concept</t>
-  </si>
-  <si>
-    <t>Marketing</t>
-  </si>
-  <si>
-    <t>marketing, channel marketing, sales, go to market strategy</t>
-  </si>
-  <si>
-    <t>Business Modeling</t>
-  </si>
-  <si>
-    <t>business model, business model canvas, go to market plan, venture forming</t>
-  </si>
-  <si>
-    <t>Managerial Decision Making</t>
-  </si>
-  <si>
-    <t>group, project, team, management, project management, lead, decision-making</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Legal </t>
-  </si>
-  <si>
-    <t>legal matters, contracts, intellectual property, copyright, agreements, trade secrets, patents, license</t>
-  </si>
-  <si>
-    <t>Financial Decision Making</t>
-  </si>
-  <si>
-    <t>financial, venture capital, financial modelling, investment/investing, revenue, funding</t>
-  </si>
-  <si>
-    <t>Observational skills</t>
-  </si>
-  <si>
-    <t>observing, questioning, seeing, sensing</t>
-  </si>
-  <si>
-    <t>Creativity skills</t>
-  </si>
-  <si>
-    <t>associating, creative thinking, innovative thinking, idea generation, prototyping, experimenting</t>
-  </si>
-  <si>
-    <t>Problem solving skills</t>
-  </si>
-  <si>
-    <t>problem solving, problem identification, opportunity identification</t>
-  </si>
-  <si>
-    <t>Communication skills</t>
-  </si>
-  <si>
-    <t>presentation, present, pitch, communication, visual thinking, sketch, map, write, design, storytelling</t>
-  </si>
-  <si>
-    <t>Decision-making skills</t>
-  </si>
-  <si>
-    <t>analytical thinking, critical thinking, assess, evaluate</t>
-  </si>
-  <si>
-    <t>Planning and project managing skills</t>
-  </si>
-  <si>
-    <t>testing, process mapping, roadmap, project manage</t>
-  </si>
-  <si>
-    <t>Networking skills</t>
-  </si>
-  <si>
-    <t>team forming, team building, connections, contacts, relationships</t>
-  </si>
-  <si>
-    <t>Negotiating skills</t>
-  </si>
-  <si>
-    <t>team management, persuasive, empathy, stakeholder engagement</t>
-  </si>
-  <si>
-    <t>Self-Aware</t>
-  </si>
-  <si>
-    <t>risk-tolerant, open, take initiative, enterprising, committed, traits</t>
-  </si>
-  <si>
-    <t>Enterprising Mindset</t>
-  </si>
-  <si>
-    <t>curiosity, self-motivated, experimental, confident, competitive, pro-active</t>
-  </si>
-  <si>
-    <t>Self-Directed</t>
-  </si>
-  <si>
-    <t>readings, supplemental activities, goal oriented, take initiative, independent, self-starter</t>
-  </si>
-  <si>
-    <t>Teamwork</t>
-  </si>
-  <si>
-    <t>networking, empathy, group management, co-founders, peers, colleagues, partners</t>
-  </si>
-  <si>
-    <t>Uncertainty Management</t>
-  </si>
-  <si>
-    <t>uncertainty, ambiguity, navigation, unfamiliar, volitility, risk, complexity</t>
-  </si>
-  <si>
-    <t>LaunchWeek</t>
-  </si>
-  <si>
-    <t>market research, primary research, secondary research, consumer research, competitor research</t>
-  </si>
-  <si>
-    <t>marketing, channel marketing, sales, go to market strategy, customer discovery, customer validation</t>
-  </si>
-  <si>
-    <t>legal matters, contracts, intellectual property, copyright, agreements, trade secrets</t>
-  </si>
-  <si>
-    <t>Enterprising Traits</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="5">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <sz val="12"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="4" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="4" tint="0.39997558519241921"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="4" tint="0.3999755851924192"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="4" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="4" tint="-0.499984740745262"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -301,15 +102,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -337,14 +138,74 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -644,69 +505,105 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="39.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="117.1640625" bestFit="1" customWidth="1"/>
+    <col width="39.83203125" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="117.1640625" bestFit="1" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Comptency</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>keyword</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>e@UBCV</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>e@UBCO</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>UBC Social Enterprise Club</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>eProjects UBC</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Enactus UBC</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Innovation UBC Hub</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Summit Leaders</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>UBC Sauder LIFT</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>UBC MBA Innovation &amp; Entrepreneurship club</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Innovation on Board</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Engineers without borders</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Startup Pitch Competition event: UBC SOAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="inlineStr">
+        <is>
+          <t>Entrepreneurial Mindset</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>entrepreneur types, traits, openness, curiosity, growth mindset, resoucefulness, resilience, grit</t>
+        </is>
       </c>
       <c r="C2" t="b">
         <v>1</v>
@@ -745,12 +642,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
+    <row r="3">
+      <c r="A3" s="6" t="inlineStr">
+        <is>
+          <t>Opportunity Recognition</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>opportunity identification, opportunity recognition, need finding, problem identification</t>
+        </is>
       </c>
       <c r="C3" t="b">
         <v>1</v>
@@ -789,12 +690,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
+    <row r="4">
+      <c r="A4" s="6" t="inlineStr">
+        <is>
+          <t>Market Research</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>market research, primary research, secondary research, consumer research, competitor research, customer discovery, customer validation</t>
+        </is>
       </c>
       <c r="C4" t="b">
         <v>0</v>
@@ -833,12 +738,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
+    <row r="5">
+      <c r="A5" s="6" t="inlineStr">
+        <is>
+          <t>Product Development</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>product research, prototype, MVP, product, service development, technology research, proof of concept</t>
+        </is>
       </c>
       <c r="C5" t="b">
         <v>1</v>
@@ -877,12 +786,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
-        <v>23</v>
+    <row r="6">
+      <c r="A6" s="6" t="inlineStr">
+        <is>
+          <t>Marketing</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>marketing, channel marketing, sales, go to market strategy</t>
+        </is>
       </c>
       <c r="C6" t="b">
         <v>0</v>
@@ -921,12 +834,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" t="s">
-        <v>25</v>
+    <row r="7">
+      <c r="A7" s="6" t="inlineStr">
+        <is>
+          <t>Business Modeling</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>business model, business model canvas, go to market plan, venture forming</t>
+        </is>
       </c>
       <c r="C7" t="b">
         <v>1</v>
@@ -965,12 +882,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" t="s">
-        <v>27</v>
+    <row r="8">
+      <c r="A8" s="6" t="inlineStr">
+        <is>
+          <t>Managerial Decision Making</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>group, project, team, management, project management, lead, decision-making</t>
+        </is>
       </c>
       <c r="C8" t="b">
         <v>1</v>
@@ -1009,12 +930,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" t="s">
-        <v>29</v>
+    <row r="9">
+      <c r="A9" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Legal </t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>legal matters, contracts, intellectual property, copyright, agreements, trade secrets, patents, license</t>
+        </is>
       </c>
       <c r="C9" t="b">
         <v>0</v>
@@ -1053,12 +978,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" t="s">
-        <v>31</v>
+    <row r="10">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>Financial Decision Making</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>financial, venture capital, financial modelling, investment/investing, revenue, funding</t>
+        </is>
       </c>
       <c r="C10" t="b">
         <v>0</v>
@@ -1097,12 +1026,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" t="s">
-        <v>33</v>
+    <row r="11">
+      <c r="A11" s="4" t="inlineStr">
+        <is>
+          <t>Observational skills</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>observing, questioning, seeing, sensing</t>
+        </is>
       </c>
       <c r="C11" t="b">
         <v>1</v>
@@ -1141,12 +1074,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" t="s">
-        <v>35</v>
+    <row r="12">
+      <c r="A12" s="4" t="inlineStr">
+        <is>
+          <t>Creativity skills</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>associating, creative thinking, innovative thinking, idea generation, prototyping, experimenting</t>
+        </is>
       </c>
       <c r="C12" t="b">
         <v>1</v>
@@ -1185,12 +1122,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" t="s">
-        <v>37</v>
+    <row r="13">
+      <c r="A13" s="4" t="inlineStr">
+        <is>
+          <t>Problem solving skills</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>problem solving, problem identification, opportunity identification</t>
+        </is>
       </c>
       <c r="C13" t="b">
         <v>0</v>
@@ -1229,12 +1170,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" t="s">
-        <v>39</v>
+    <row r="14">
+      <c r="A14" s="4" t="inlineStr">
+        <is>
+          <t>Communication skills</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>presentation, present, pitch, communication, visual thinking, sketch, map, write, design, storytelling</t>
+        </is>
       </c>
       <c r="C14" t="b">
         <v>1</v>
@@ -1273,12 +1218,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" t="s">
-        <v>41</v>
+    <row r="15">
+      <c r="A15" s="4" t="inlineStr">
+        <is>
+          <t>Decision-making skills</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>analytical thinking, critical thinking, assess, evaluate</t>
+        </is>
       </c>
       <c r="C15" t="b">
         <v>1</v>
@@ -1317,12 +1266,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" t="s">
-        <v>43</v>
+    <row r="16">
+      <c r="A16" s="4" t="inlineStr">
+        <is>
+          <t>Planning and project managing skills</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>testing, process mapping, roadmap, project manage</t>
+        </is>
       </c>
       <c r="C16" t="b">
         <v>1</v>
@@ -1361,12 +1314,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" t="s">
-        <v>45</v>
+    <row r="17">
+      <c r="A17" s="4" t="inlineStr">
+        <is>
+          <t>Networking skills</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>team forming, team building, connections, contacts, relationships</t>
+        </is>
       </c>
       <c r="C17" t="b">
         <v>1</v>
@@ -1405,12 +1362,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" t="s">
-        <v>47</v>
+    <row r="18">
+      <c r="A18" s="4" t="inlineStr">
+        <is>
+          <t>Negotiating skills</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>team management, persuasive, empathy, stakeholder engagement</t>
+        </is>
       </c>
       <c r="C18" t="b">
         <v>1</v>
@@ -1449,12 +1410,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" t="s">
-        <v>49</v>
+    <row r="19">
+      <c r="A19" s="5" t="inlineStr">
+        <is>
+          <t>Self-Aware</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>risk-tolerant, open, take initiative, enterprising, committed, traits</t>
+        </is>
       </c>
       <c r="C19" t="b">
         <v>1</v>
@@ -1493,12 +1458,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B20" t="s">
-        <v>51</v>
+    <row r="20">
+      <c r="A20" s="5" t="inlineStr">
+        <is>
+          <t>Enterprising Traits</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>curiosity, self-motivated, experimental, confident, competitive, pro-active</t>
+        </is>
       </c>
       <c r="C20" t="b">
         <v>1</v>
@@ -1537,12 +1506,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B21" t="s">
-        <v>53</v>
+    <row r="21">
+      <c r="A21" s="5" t="inlineStr">
+        <is>
+          <t>Self-Directed</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>readings, supplemental activities, goal oriented, take initiative, independent, self-starter</t>
+        </is>
       </c>
       <c r="C21" t="b">
         <v>1</v>
@@ -1581,12 +1554,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22" t="s">
-        <v>55</v>
+    <row r="22">
+      <c r="A22" s="5" t="inlineStr">
+        <is>
+          <t>Teamwork</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>networking, empathy, group management, co-founders, peers, colleagues, partners</t>
+        </is>
       </c>
       <c r="C22" t="b">
         <v>1</v>
@@ -1625,12 +1602,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B23" t="s">
-        <v>57</v>
+    <row r="23">
+      <c r="A23" s="5" t="inlineStr">
+        <is>
+          <t>Uncertainty Management</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>uncertainty, ambiguity, navigation, unfamiliar, volitility, risk, complexity</t>
+        </is>
       </c>
       <c r="C23" t="b">
         <v>1</v>
@@ -1671,165 +1652,231 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:N1048576">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="false">
+    <cfRule type="containsText" priority="2" operator="containsText" dxfId="1" text="false">
       <formula>NOT(ISERROR(SEARCH("false",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="true">
+    <cfRule type="containsText" priority="1" operator="containsText" dxfId="0" text="true">
       <formula>NOT(ISERROR(SEARCH("true",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C1" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D1" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C1" r:id="rId1"/>
+    <hyperlink ref="D1" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="A1" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>58</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>e@UBCV</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>e@UBCO</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>UBC Social Enterprise Club</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>eProjects UBC</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Enactus UBC</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Innovation UBC Hub</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Summit Leaders</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>UBC Sauder LIFT</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>UBC MBA Innovation &amp; Entrepreneurship club</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Innovation on Board</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Engineers without borders</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Startup Pitch Competition event: UBC SOAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>LaunchWeek</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="A1" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:N23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
+    <row r="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>Comptency</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>keyword</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>e@UBCV</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>e@UBCO</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>UBC Social Enterprise Club</t>
+        </is>
+      </c>
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>eProjects UBC</t>
+        </is>
+      </c>
+      <c r="G1" s="3" t="inlineStr">
+        <is>
+          <t>Enactus UBC</t>
+        </is>
+      </c>
+      <c r="H1" s="3" t="inlineStr">
+        <is>
+          <t>Innovation UBC Hub</t>
+        </is>
+      </c>
+      <c r="I1" s="3" t="inlineStr">
+        <is>
+          <t>Summit Leaders</t>
+        </is>
+      </c>
+      <c r="J1" s="3" t="inlineStr">
+        <is>
+          <t>UBC Sauder LIFT</t>
+        </is>
+      </c>
+      <c r="K1" s="3" t="inlineStr">
+        <is>
+          <t>UBC MBA Innovation &amp; Entrepreneurship club</t>
+        </is>
+      </c>
+      <c r="L1" s="3" t="inlineStr">
+        <is>
+          <t>Innovation on Board</t>
+        </is>
+      </c>
+      <c r="M1" s="3" t="inlineStr">
+        <is>
+          <t>Engineers without borders</t>
+        </is>
+      </c>
+      <c r="N1" s="3" t="inlineStr">
+        <is>
+          <t>Startup Pitch Competition event: UBC SOAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Entrepreneurial Mindset</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>entrepreneur types, traits, openness, curiosity, growth mindset, resoucefulness, resilience, grit</t>
+        </is>
       </c>
       <c r="C2" t="b">
         <v>1</v>
@@ -1868,12 +1915,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Opportunity Recognition</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>opportunity identification, opportunity recognition, need finding, problem identification</t>
+        </is>
       </c>
       <c r="C3" t="b">
         <v>1</v>
@@ -1912,12 +1963,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>59</v>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Market Research</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>market research, primary research, secondary research, consumer research, competitor research</t>
+        </is>
       </c>
       <c r="C4" t="b">
         <v>0</v>
@@ -1956,12 +2011,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Product Development</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>product research, prototype, MVP, product, service development, technology research, proof of concept</t>
+        </is>
       </c>
       <c r="C5" t="b">
         <v>1</v>
@@ -2000,12 +2059,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
-        <v>60</v>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Marketing</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>marketing, channel marketing, sales, go to market strategy, customer discovery, customer validation</t>
+        </is>
       </c>
       <c r="C6" t="b">
         <v>0</v>
@@ -2044,12 +2107,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" t="s">
-        <v>25</v>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Business Modeling</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>business model, business model canvas, go to market plan, venture forming</t>
+        </is>
       </c>
       <c r="C7" t="b">
         <v>1</v>
@@ -2088,12 +2155,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" t="s">
-        <v>27</v>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Managerial Decision Making</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>group, project, team, management, project management, lead, decision-making</t>
+        </is>
       </c>
       <c r="C8" t="b">
         <v>1</v>
@@ -2132,12 +2203,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" t="s">
-        <v>61</v>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Legal </t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>legal matters, contracts, intellectual property, copyright, agreements, trade secrets</t>
+        </is>
       </c>
       <c r="C9" t="b">
         <v>0</v>
@@ -2176,12 +2251,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" t="s">
-        <v>31</v>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Financial Decision Making</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>financial, venture capital, financial modelling, investment/investing, revenue, funding</t>
+        </is>
       </c>
       <c r="C10" t="b">
         <v>0</v>
@@ -2220,12 +2299,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" t="s">
-        <v>33</v>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Observational skills</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>observing, questioning, seeing, sensing</t>
+        </is>
       </c>
       <c r="C11" t="b">
         <v>1</v>
@@ -2264,12 +2347,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" t="s">
-        <v>35</v>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Creativity skills</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>associating, creative thinking, innovative thinking, idea generation, prototyping, experimenting</t>
+        </is>
       </c>
       <c r="C12" t="b">
         <v>1</v>
@@ -2308,12 +2395,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" t="s">
-        <v>37</v>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Problem solving skills</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>problem solving, problem identification, opportunity identification</t>
+        </is>
       </c>
       <c r="C13" t="b">
         <v>0</v>
@@ -2352,12 +2443,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" t="s">
-        <v>39</v>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Communication skills</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>presentation, present, pitch, communication, visual thinking, sketch, map, write, design, storytelling</t>
+        </is>
       </c>
       <c r="C14" t="b">
         <v>1</v>
@@ -2396,12 +2491,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" t="s">
-        <v>41</v>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Decision-making skills</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>analytical thinking, critical thinking, assess, evaluate</t>
+        </is>
       </c>
       <c r="C15" t="b">
         <v>1</v>
@@ -2440,12 +2539,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" t="s">
-        <v>43</v>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Planning and project managing skills</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>testing, process mapping, roadmap, project manage</t>
+        </is>
       </c>
       <c r="C16" t="b">
         <v>1</v>
@@ -2484,12 +2587,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" t="s">
-        <v>45</v>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Networking skills</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>team forming, team building, connections, contacts, relationships</t>
+        </is>
       </c>
       <c r="C17" t="b">
         <v>1</v>
@@ -2528,12 +2635,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" t="s">
-        <v>47</v>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Negotiating skills</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>team management, persuasive, empathy, stakeholder engagement</t>
+        </is>
       </c>
       <c r="C18" t="b">
         <v>1</v>
@@ -2572,12 +2683,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" t="s">
-        <v>49</v>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Self-Aware</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>risk-tolerant, open, take initiative, enterprising, committed, traits</t>
+        </is>
       </c>
       <c r="C19" t="b">
         <v>1</v>
@@ -2616,12 +2731,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>50</v>
-      </c>
-      <c r="B20" t="s">
-        <v>51</v>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Enterprising Mindset</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>curiosity, self-motivated, experimental, confident, competitive, pro-active</t>
+        </is>
       </c>
       <c r="C20" t="b">
         <v>1</v>
@@ -2660,12 +2779,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>52</v>
-      </c>
-      <c r="B21" t="s">
-        <v>53</v>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Self-Directed</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>readings, supplemental activities, goal oriented, take initiative, independent, self-starter</t>
+        </is>
       </c>
       <c r="C21" t="b">
         <v>1</v>
@@ -2704,12 +2827,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22" t="s">
-        <v>55</v>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Teamwork</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>networking, empathy, group management, co-founders, peers, colleagues, partners</t>
+        </is>
       </c>
       <c r="C22" t="b">
         <v>1</v>
@@ -2748,12 +2875,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>56</v>
-      </c>
-      <c r="B23" t="s">
-        <v>57</v>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Uncertainty Management</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>uncertainty, ambiguity, navigation, unfamiliar, volitility, risk, complexity</t>
+        </is>
       </c>
       <c r="C23" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
add the competency to the keywords as well to ease the score selection process
</commit_message>
<xml_diff>
--- a/data/cocurricular_competencies.xlsx
+++ b/data/cocurricular_competencies.xlsx
@@ -1,62 +1,294 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/radman/Desktop/All/projects/EER/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9999B8FB-EB3E-C949-B46C-6CAC553F258C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Modified keyword Classification" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Modified keyword Classification" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="74">
+  <si>
+    <t>Comptency</t>
+  </si>
+  <si>
+    <t>keyword</t>
+  </si>
+  <si>
+    <t>e@UBCV</t>
+  </si>
+  <si>
+    <t>e@UBCO</t>
+  </si>
+  <si>
+    <t>UBC Social Enterprise Club</t>
+  </si>
+  <si>
+    <t>eProjects UBC</t>
+  </si>
+  <si>
+    <t>Enactus UBC</t>
+  </si>
+  <si>
+    <t>Innovation UBC Hub</t>
+  </si>
+  <si>
+    <t>Summit Leaders</t>
+  </si>
+  <si>
+    <t>UBC Sauder LIFT</t>
+  </si>
+  <si>
+    <t>UBC MBA Innovation &amp; Entrepreneurship club</t>
+  </si>
+  <si>
+    <t>Innovation on Board</t>
+  </si>
+  <si>
+    <t>Engineers without borders</t>
+  </si>
+  <si>
+    <t>Startup Pitch Competition event: UBC SOAR</t>
+  </si>
+  <si>
+    <t>Entrepreneurial Mindset</t>
+  </si>
+  <si>
+    <t>entrepreneur types, traits, openness, curiosity, growth mindset, resoucefulness, resilience, grit</t>
+  </si>
+  <si>
+    <t>Opportunity Recognition</t>
+  </si>
+  <si>
+    <t>opportunity identification, opportunity recognition, need finding, problem identification</t>
+  </si>
+  <si>
+    <t>Market Research</t>
+  </si>
+  <si>
+    <t>market research, primary research, secondary research, consumer research, competitor research, customer discovery, customer validation</t>
+  </si>
+  <si>
+    <t>Product Development</t>
+  </si>
+  <si>
+    <t>product research, prototype, MVP, product, service development, technology research, proof of concept</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>marketing, channel marketing, sales, go to market strategy</t>
+  </si>
+  <si>
+    <t>Business Modeling</t>
+  </si>
+  <si>
+    <t>business model, business model canvas, go to market plan, venture forming</t>
+  </si>
+  <si>
+    <t>Managerial Decision Making</t>
+  </si>
+  <si>
+    <t>group, project, team, management, project management, lead, decision-making</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Legal </t>
+  </si>
+  <si>
+    <t>Financial Decision Making</t>
+  </si>
+  <si>
+    <t>financial, venture capital, financial modelling, investment/investing, revenue, funding</t>
+  </si>
+  <si>
+    <t>Observational skills</t>
+  </si>
+  <si>
+    <t>observing, questioning, seeing, sensing</t>
+  </si>
+  <si>
+    <t>Creativity skills</t>
+  </si>
+  <si>
+    <t>associating, creative thinking, innovative thinking, idea generation, prototyping, experimenting</t>
+  </si>
+  <si>
+    <t>Problem solving skills</t>
+  </si>
+  <si>
+    <t>problem solving, problem identification, opportunity identification</t>
+  </si>
+  <si>
+    <t>Communication skills</t>
+  </si>
+  <si>
+    <t>presentation, present, pitch, communication, visual thinking, sketch, map, write, design, storytelling</t>
+  </si>
+  <si>
+    <t>Decision-making skills</t>
+  </si>
+  <si>
+    <t>analytical thinking, critical thinking, assess, evaluate</t>
+  </si>
+  <si>
+    <t>Planning and project managing skills</t>
+  </si>
+  <si>
+    <t>testing, process mapping, roadmap, project manage</t>
+  </si>
+  <si>
+    <t>Networking skills</t>
+  </si>
+  <si>
+    <t>team forming, team building, connections, contacts, relationships</t>
+  </si>
+  <si>
+    <t>Negotiating skills</t>
+  </si>
+  <si>
+    <t>team management, persuasive, empathy, stakeholder engagement</t>
+  </si>
+  <si>
+    <t>Self-Aware</t>
+  </si>
+  <si>
+    <t>risk-tolerant, open, take initiative, enterprising, committed, traits</t>
+  </si>
+  <si>
+    <t>Enterprising Traits</t>
+  </si>
+  <si>
+    <t>curiosity, self-motivated, experimental, confident, competitive, pro-active</t>
+  </si>
+  <si>
+    <t>Self-Directed</t>
+  </si>
+  <si>
+    <t>readings, supplemental activities, goal oriented, take initiative, independent, self-starter</t>
+  </si>
+  <si>
+    <t>Teamwork</t>
+  </si>
+  <si>
+    <t>networking, empathy, group management, co-founders, peers, colleagues, partners</t>
+  </si>
+  <si>
+    <t>Uncertainty Management</t>
+  </si>
+  <si>
+    <t>uncertainty, ambiguity, navigation, unfamiliar, volitility, risk, complexity</t>
+  </si>
+  <si>
+    <t>LaunchWeek</t>
+  </si>
+  <si>
+    <t>market research, primary research, secondary research, consumer research, competitor research</t>
+  </si>
+  <si>
+    <t>marketing, channel marketing, sales, go to market strategy, customer discovery, customer validation</t>
+  </si>
+  <si>
+    <t>legal matters, contracts, intellectual property, copyright, agreements, trade secrets</t>
+  </si>
+  <si>
+    <t>Enterprising Mindset</t>
+  </si>
+  <si>
+    <t>Entrepreneurial Mindset, entrepreneur types, traits, openness, curiosity, growth mindset, resoucefulness, resilience, grit</t>
+  </si>
+  <si>
+    <t>Opportunity Recognition, opportunity identification, opportunity recognition, need finding, problem identification</t>
+  </si>
+  <si>
+    <t>Product Development, product research, prototype, MVP, product, service development, technology research, proof of concept</t>
+  </si>
+  <si>
+    <t>Managerial Decision Making, group, project, team, management, project management, lead, decision-making</t>
+  </si>
+  <si>
+    <t>legal, contracts, intellectual property, copyright, agreements, trade secrets, patents, license</t>
+  </si>
+  <si>
+    <t>creative, associating, innovative thinking, idea generation, prototyping, experimenting</t>
+  </si>
+  <si>
+    <t>Decision-making, analytical thinking, critical thinking, assess, evaluate</t>
+  </si>
+  <si>
+    <t>planning, managing, testing, process mapping, roadmap, project manage</t>
+  </si>
+  <si>
+    <t>networking, team forming, team building, connections, contacts, relationships</t>
+  </si>
+  <si>
+    <t>Negotiating, team management, persuasive, empathy, stakeholder engagement</t>
+  </si>
+  <si>
+    <t>Self-Directed, readings, supplemental activities, goal oriented, take initiative, independent, self-starter</t>
+  </si>
+  <si>
+    <t>teamwork, empathy, group management, co-founders, peers, colleagues, partners</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
-      <sz val="12"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="4" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="4" tint="-0.249977111117893"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="4" tint="0.39997558519241921"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="4" tint="0.3999755851924192"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="4" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="4" tint="-0.499984740745262"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -102,20 +334,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -126,86 +368,16 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -505,105 +677,69 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col width="39.83203125" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="117.1640625" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col min="1" max="1" width="39.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="117.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="inlineStr">
-        <is>
-          <t>Comptency</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>keyword</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>e@UBCV</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>e@UBCO</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>UBC Social Enterprise Club</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>eProjects UBC</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Enactus UBC</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Innovation UBC Hub</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Summit Leaders</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>UBC Sauder LIFT</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>UBC MBA Innovation &amp; Entrepreneurship club</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Innovation on Board</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Engineers without borders</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Startup Pitch Competition event: UBC SOAR</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="6" t="inlineStr">
-        <is>
-          <t>Entrepreneurial Mindset</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>entrepreneur types, traits, openness, curiosity, growth mindset, resoucefulness, resilience, grit</t>
-        </is>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
@@ -642,16 +778,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="6" t="inlineStr">
-        <is>
-          <t>Opportunity Recognition</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>opportunity identification, opportunity recognition, need finding, problem identification</t>
-        </is>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
       </c>
       <c r="C3" t="b">
         <v>1</v>
@@ -690,16 +822,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="6" t="inlineStr">
-        <is>
-          <t>Market Research</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>market research, primary research, secondary research, consumer research, competitor research, customer discovery, customer validation</t>
-        </is>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
@@ -738,16 +866,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="6" t="inlineStr">
-        <is>
-          <t>Product Development</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>product research, prototype, MVP, product, service development, technology research, proof of concept</t>
-        </is>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>64</v>
       </c>
       <c r="C5" t="b">
         <v>1</v>
@@ -786,16 +910,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="6" t="inlineStr">
-        <is>
-          <t>Marketing</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>marketing, channel marketing, sales, go to market strategy</t>
-        </is>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
       </c>
       <c r="C6" t="b">
         <v>0</v>
@@ -834,16 +954,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="6" t="inlineStr">
-        <is>
-          <t>Business Modeling</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>business model, business model canvas, go to market plan, venture forming</t>
-        </is>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
       </c>
       <c r="C7" t="b">
         <v>1</v>
@@ -882,16 +998,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="6" t="inlineStr">
-        <is>
-          <t>Managerial Decision Making</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>group, project, team, management, project management, lead, decision-making</t>
-        </is>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>65</v>
       </c>
       <c r="C8" t="b">
         <v>1</v>
@@ -930,16 +1042,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Legal </t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>legal matters, contracts, intellectual property, copyright, agreements, trade secrets, patents, license</t>
-        </is>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>66</v>
       </c>
       <c r="C9" t="b">
         <v>0</v>
@@ -978,16 +1086,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="6" t="inlineStr">
-        <is>
-          <t>Financial Decision Making</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>financial, venture capital, financial modelling, investment/investing, revenue, funding</t>
-        </is>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
       </c>
       <c r="C10" t="b">
         <v>0</v>
@@ -1026,16 +1130,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="4" t="inlineStr">
-        <is>
-          <t>Observational skills</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>observing, questioning, seeing, sensing</t>
-        </is>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
       </c>
       <c r="C11" t="b">
         <v>1</v>
@@ -1074,16 +1174,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="4" t="inlineStr">
-        <is>
-          <t>Creativity skills</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>associating, creative thinking, innovative thinking, idea generation, prototyping, experimenting</t>
-        </is>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>67</v>
       </c>
       <c r="C12" t="b">
         <v>1</v>
@@ -1122,16 +1218,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="4" t="inlineStr">
-        <is>
-          <t>Problem solving skills</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>problem solving, problem identification, opportunity identification</t>
-        </is>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
       </c>
       <c r="C13" t="b">
         <v>0</v>
@@ -1170,16 +1262,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="4" t="inlineStr">
-        <is>
-          <t>Communication skills</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>presentation, present, pitch, communication, visual thinking, sketch, map, write, design, storytelling</t>
-        </is>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
       </c>
       <c r="C14" t="b">
         <v>1</v>
@@ -1218,16 +1306,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="4" t="inlineStr">
-        <is>
-          <t>Decision-making skills</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>analytical thinking, critical thinking, assess, evaluate</t>
-        </is>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>68</v>
       </c>
       <c r="C15" t="b">
         <v>1</v>
@@ -1266,16 +1350,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="4" t="inlineStr">
-        <is>
-          <t>Planning and project managing skills</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>testing, process mapping, roadmap, project manage</t>
-        </is>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" t="s">
+        <v>69</v>
       </c>
       <c r="C16" t="b">
         <v>1</v>
@@ -1314,16 +1394,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="4" t="inlineStr">
-        <is>
-          <t>Networking skills</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>team forming, team building, connections, contacts, relationships</t>
-        </is>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" t="s">
+        <v>70</v>
       </c>
       <c r="C17" t="b">
         <v>1</v>
@@ -1362,16 +1438,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="4" t="inlineStr">
-        <is>
-          <t>Negotiating skills</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>team management, persuasive, empathy, stakeholder engagement</t>
-        </is>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" t="s">
+        <v>71</v>
       </c>
       <c r="C18" t="b">
         <v>1</v>
@@ -1410,16 +1482,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="5" t="inlineStr">
-        <is>
-          <t>Self-Aware</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>risk-tolerant, open, take initiative, enterprising, committed, traits</t>
-        </is>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" t="s">
+        <v>48</v>
       </c>
       <c r="C19" t="b">
         <v>1</v>
@@ -1458,16 +1526,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="5" t="inlineStr">
-        <is>
-          <t>Enterprising Traits</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>curiosity, self-motivated, experimental, confident, competitive, pro-active</t>
-        </is>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" t="s">
+        <v>50</v>
       </c>
       <c r="C20" t="b">
         <v>1</v>
@@ -1506,16 +1570,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="5" t="inlineStr">
-        <is>
-          <t>Self-Directed</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>readings, supplemental activities, goal oriented, take initiative, independent, self-starter</t>
-        </is>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" t="s">
+        <v>72</v>
       </c>
       <c r="C21" t="b">
         <v>1</v>
@@ -1554,16 +1614,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="5" t="inlineStr">
-        <is>
-          <t>Teamwork</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>networking, empathy, group management, co-founders, peers, colleagues, partners</t>
-        </is>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" t="s">
+        <v>73</v>
       </c>
       <c r="C22" t="b">
         <v>1</v>
@@ -1602,16 +1658,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="5" t="inlineStr">
-        <is>
-          <t>Uncertainty Management</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>uncertainty, ambiguity, navigation, unfamiliar, volitility, risk, complexity</t>
-        </is>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" t="s">
+        <v>56</v>
       </c>
       <c r="C23" t="b">
         <v>1</v>
@@ -1652,231 +1704,165 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:N1048576">
-    <cfRule type="containsText" priority="2" operator="containsText" dxfId="1" text="false">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="true">
+      <formula>NOT(ISERROR(SEARCH("true",C1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="false">
       <formula>NOT(ISERROR(SEARCH("false",C1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" priority="1" operator="containsText" dxfId="0" text="true">
-      <formula>NOT(ISERROR(SEARCH("true",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C1" r:id="rId1"/>
-    <hyperlink ref="D1" r:id="rId2"/>
+    <hyperlink ref="C1" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D1" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:A1048576"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>e@UBCV</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>e@UBCO</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>UBC Social Enterprise Club</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>eProjects UBC</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Enactus UBC</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Innovation UBC Hub</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Summit Leaders</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>UBC Sauder LIFT</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>UBC MBA Innovation &amp; Entrepreneurship club</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Innovation on Board</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Engineers without borders</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Startup Pitch Competition event: UBC SOAR</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>LaunchWeek</t>
-        </is>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1"/>
-    <hyperlink ref="A2" r:id="rId2"/>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:N23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="3" t="inlineStr">
-        <is>
-          <t>Comptency</t>
-        </is>
-      </c>
-      <c r="B1" s="3" t="inlineStr">
-        <is>
-          <t>keyword</t>
-        </is>
-      </c>
-      <c r="C1" s="3" t="inlineStr">
-        <is>
-          <t>e@UBCV</t>
-        </is>
-      </c>
-      <c r="D1" s="3" t="inlineStr">
-        <is>
-          <t>e@UBCO</t>
-        </is>
-      </c>
-      <c r="E1" s="3" t="inlineStr">
-        <is>
-          <t>UBC Social Enterprise Club</t>
-        </is>
-      </c>
-      <c r="F1" s="3" t="inlineStr">
-        <is>
-          <t>eProjects UBC</t>
-        </is>
-      </c>
-      <c r="G1" s="3" t="inlineStr">
-        <is>
-          <t>Enactus UBC</t>
-        </is>
-      </c>
-      <c r="H1" s="3" t="inlineStr">
-        <is>
-          <t>Innovation UBC Hub</t>
-        </is>
-      </c>
-      <c r="I1" s="3" t="inlineStr">
-        <is>
-          <t>Summit Leaders</t>
-        </is>
-      </c>
-      <c r="J1" s="3" t="inlineStr">
-        <is>
-          <t>UBC Sauder LIFT</t>
-        </is>
-      </c>
-      <c r="K1" s="3" t="inlineStr">
-        <is>
-          <t>UBC MBA Innovation &amp; Entrepreneurship club</t>
-        </is>
-      </c>
-      <c r="L1" s="3" t="inlineStr">
-        <is>
-          <t>Innovation on Board</t>
-        </is>
-      </c>
-      <c r="M1" s="3" t="inlineStr">
-        <is>
-          <t>Engineers without borders</t>
-        </is>
-      </c>
-      <c r="N1" s="3" t="inlineStr">
-        <is>
-          <t>Startup Pitch Competition event: UBC SOAR</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Entrepreneurial Mindset</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>entrepreneur types, traits, openness, curiosity, growth mindset, resoucefulness, resilience, grit</t>
-        </is>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
@@ -1915,16 +1901,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Opportunity Recognition</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>opportunity identification, opportunity recognition, need finding, problem identification</t>
-        </is>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
       </c>
       <c r="C3" t="b">
         <v>1</v>
@@ -1963,16 +1945,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Market Research</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>market research, primary research, secondary research, consumer research, competitor research</t>
-        </is>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>58</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
@@ -2011,16 +1989,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Product Development</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>product research, prototype, MVP, product, service development, technology research, proof of concept</t>
-        </is>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
       </c>
       <c r="C5" t="b">
         <v>1</v>
@@ -2059,16 +2033,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Marketing</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>marketing, channel marketing, sales, go to market strategy, customer discovery, customer validation</t>
-        </is>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>59</v>
       </c>
       <c r="C6" t="b">
         <v>0</v>
@@ -2107,16 +2077,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Business Modeling</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>business model, business model canvas, go to market plan, venture forming</t>
-        </is>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
       </c>
       <c r="C7" t="b">
         <v>1</v>
@@ -2155,16 +2121,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Managerial Decision Making</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>group, project, team, management, project management, lead, decision-making</t>
-        </is>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
       </c>
       <c r="C8" t="b">
         <v>1</v>
@@ -2203,16 +2165,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Legal </t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>legal matters, contracts, intellectual property, copyright, agreements, trade secrets</t>
-        </is>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>60</v>
       </c>
       <c r="C9" t="b">
         <v>0</v>
@@ -2251,16 +2209,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Financial Decision Making</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>financial, venture capital, financial modelling, investment/investing, revenue, funding</t>
-        </is>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
       </c>
       <c r="C10" t="b">
         <v>0</v>
@@ -2299,16 +2253,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Observational skills</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>observing, questioning, seeing, sensing</t>
-        </is>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
       </c>
       <c r="C11" t="b">
         <v>1</v>
@@ -2347,16 +2297,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Creativity skills</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>associating, creative thinking, innovative thinking, idea generation, prototyping, experimenting</t>
-        </is>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
       </c>
       <c r="C12" t="b">
         <v>1</v>
@@ -2395,16 +2341,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Problem solving skills</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>problem solving, problem identification, opportunity identification</t>
-        </is>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
       </c>
       <c r="C13" t="b">
         <v>0</v>
@@ -2443,16 +2385,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Communication skills</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>presentation, present, pitch, communication, visual thinking, sketch, map, write, design, storytelling</t>
-        </is>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
       </c>
       <c r="C14" t="b">
         <v>1</v>
@@ -2491,16 +2429,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Decision-making skills</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>analytical thinking, critical thinking, assess, evaluate</t>
-        </is>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>40</v>
       </c>
       <c r="C15" t="b">
         <v>1</v>
@@ -2539,16 +2473,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Planning and project managing skills</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>testing, process mapping, roadmap, project manage</t>
-        </is>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" t="s">
+        <v>42</v>
       </c>
       <c r="C16" t="b">
         <v>1</v>
@@ -2587,16 +2517,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Networking skills</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>team forming, team building, connections, contacts, relationships</t>
-        </is>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" t="s">
+        <v>44</v>
       </c>
       <c r="C17" t="b">
         <v>1</v>
@@ -2635,16 +2561,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Negotiating skills</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>team management, persuasive, empathy, stakeholder engagement</t>
-        </is>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" t="s">
+        <v>46</v>
       </c>
       <c r="C18" t="b">
         <v>1</v>
@@ -2683,16 +2605,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Self-Aware</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>risk-tolerant, open, take initiative, enterprising, committed, traits</t>
-        </is>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" t="s">
+        <v>48</v>
       </c>
       <c r="C19" t="b">
         <v>1</v>
@@ -2731,16 +2649,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Enterprising Mindset</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>curiosity, self-motivated, experimental, confident, competitive, pro-active</t>
-        </is>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" t="s">
+        <v>50</v>
       </c>
       <c r="C20" t="b">
         <v>1</v>
@@ -2779,16 +2693,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Self-Directed</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>readings, supplemental activities, goal oriented, take initiative, independent, self-starter</t>
-        </is>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" t="s">
+        <v>52</v>
       </c>
       <c r="C21" t="b">
         <v>1</v>
@@ -2827,16 +2737,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Teamwork</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>networking, empathy, group management, co-founders, peers, colleagues, partners</t>
-        </is>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" t="s">
+        <v>54</v>
       </c>
       <c r="C22" t="b">
         <v>1</v>
@@ -2875,16 +2781,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Uncertainty Management</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>uncertainty, ambiguity, navigation, unfamiliar, volitility, risk, complexity</t>
-        </is>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" t="s">
+        <v>56</v>
       </c>
       <c r="C23" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
update the results of re-running the syllabi and program scripts
</commit_message>
<xml_diff>
--- a/data/cocurricular_competencies.xlsx
+++ b/data/cocurricular_competencies.xlsx
@@ -1,294 +1,62 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/radman/Desktop/All/projects/EER/data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9999B8FB-EB3E-C949-B46C-6CAC553F258C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Modified keyword Classification" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Modified keyword Classification" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="74">
-  <si>
-    <t>Comptency</t>
-  </si>
-  <si>
-    <t>keyword</t>
-  </si>
-  <si>
-    <t>e@UBCV</t>
-  </si>
-  <si>
-    <t>e@UBCO</t>
-  </si>
-  <si>
-    <t>UBC Social Enterprise Club</t>
-  </si>
-  <si>
-    <t>eProjects UBC</t>
-  </si>
-  <si>
-    <t>Enactus UBC</t>
-  </si>
-  <si>
-    <t>Innovation UBC Hub</t>
-  </si>
-  <si>
-    <t>Summit Leaders</t>
-  </si>
-  <si>
-    <t>UBC Sauder LIFT</t>
-  </si>
-  <si>
-    <t>UBC MBA Innovation &amp; Entrepreneurship club</t>
-  </si>
-  <si>
-    <t>Innovation on Board</t>
-  </si>
-  <si>
-    <t>Engineers without borders</t>
-  </si>
-  <si>
-    <t>Startup Pitch Competition event: UBC SOAR</t>
-  </si>
-  <si>
-    <t>Entrepreneurial Mindset</t>
-  </si>
-  <si>
-    <t>entrepreneur types, traits, openness, curiosity, growth mindset, resoucefulness, resilience, grit</t>
-  </si>
-  <si>
-    <t>Opportunity Recognition</t>
-  </si>
-  <si>
-    <t>opportunity identification, opportunity recognition, need finding, problem identification</t>
-  </si>
-  <si>
-    <t>Market Research</t>
-  </si>
-  <si>
-    <t>market research, primary research, secondary research, consumer research, competitor research, customer discovery, customer validation</t>
-  </si>
-  <si>
-    <t>Product Development</t>
-  </si>
-  <si>
-    <t>product research, prototype, MVP, product, service development, technology research, proof of concept</t>
-  </si>
-  <si>
-    <t>Marketing</t>
-  </si>
-  <si>
-    <t>marketing, channel marketing, sales, go to market strategy</t>
-  </si>
-  <si>
-    <t>Business Modeling</t>
-  </si>
-  <si>
-    <t>business model, business model canvas, go to market plan, venture forming</t>
-  </si>
-  <si>
-    <t>Managerial Decision Making</t>
-  </si>
-  <si>
-    <t>group, project, team, management, project management, lead, decision-making</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Legal </t>
-  </si>
-  <si>
-    <t>Financial Decision Making</t>
-  </si>
-  <si>
-    <t>financial, venture capital, financial modelling, investment/investing, revenue, funding</t>
-  </si>
-  <si>
-    <t>Observational skills</t>
-  </si>
-  <si>
-    <t>observing, questioning, seeing, sensing</t>
-  </si>
-  <si>
-    <t>Creativity skills</t>
-  </si>
-  <si>
-    <t>associating, creative thinking, innovative thinking, idea generation, prototyping, experimenting</t>
-  </si>
-  <si>
-    <t>Problem solving skills</t>
-  </si>
-  <si>
-    <t>problem solving, problem identification, opportunity identification</t>
-  </si>
-  <si>
-    <t>Communication skills</t>
-  </si>
-  <si>
-    <t>presentation, present, pitch, communication, visual thinking, sketch, map, write, design, storytelling</t>
-  </si>
-  <si>
-    <t>Decision-making skills</t>
-  </si>
-  <si>
-    <t>analytical thinking, critical thinking, assess, evaluate</t>
-  </si>
-  <si>
-    <t>Planning and project managing skills</t>
-  </si>
-  <si>
-    <t>testing, process mapping, roadmap, project manage</t>
-  </si>
-  <si>
-    <t>Networking skills</t>
-  </si>
-  <si>
-    <t>team forming, team building, connections, contacts, relationships</t>
-  </si>
-  <si>
-    <t>Negotiating skills</t>
-  </si>
-  <si>
-    <t>team management, persuasive, empathy, stakeholder engagement</t>
-  </si>
-  <si>
-    <t>Self-Aware</t>
-  </si>
-  <si>
-    <t>risk-tolerant, open, take initiative, enterprising, committed, traits</t>
-  </si>
-  <si>
-    <t>Enterprising Traits</t>
-  </si>
-  <si>
-    <t>curiosity, self-motivated, experimental, confident, competitive, pro-active</t>
-  </si>
-  <si>
-    <t>Self-Directed</t>
-  </si>
-  <si>
-    <t>readings, supplemental activities, goal oriented, take initiative, independent, self-starter</t>
-  </si>
-  <si>
-    <t>Teamwork</t>
-  </si>
-  <si>
-    <t>networking, empathy, group management, co-founders, peers, colleagues, partners</t>
-  </si>
-  <si>
-    <t>Uncertainty Management</t>
-  </si>
-  <si>
-    <t>uncertainty, ambiguity, navigation, unfamiliar, volitility, risk, complexity</t>
-  </si>
-  <si>
-    <t>LaunchWeek</t>
-  </si>
-  <si>
-    <t>market research, primary research, secondary research, consumer research, competitor research</t>
-  </si>
-  <si>
-    <t>marketing, channel marketing, sales, go to market strategy, customer discovery, customer validation</t>
-  </si>
-  <si>
-    <t>legal matters, contracts, intellectual property, copyright, agreements, trade secrets</t>
-  </si>
-  <si>
-    <t>Enterprising Mindset</t>
-  </si>
-  <si>
-    <t>Entrepreneurial Mindset, entrepreneur types, traits, openness, curiosity, growth mindset, resoucefulness, resilience, grit</t>
-  </si>
-  <si>
-    <t>Opportunity Recognition, opportunity identification, opportunity recognition, need finding, problem identification</t>
-  </si>
-  <si>
-    <t>Product Development, product research, prototype, MVP, product, service development, technology research, proof of concept</t>
-  </si>
-  <si>
-    <t>Managerial Decision Making, group, project, team, management, project management, lead, decision-making</t>
-  </si>
-  <si>
-    <t>legal, contracts, intellectual property, copyright, agreements, trade secrets, patents, license</t>
-  </si>
-  <si>
-    <t>creative, associating, innovative thinking, idea generation, prototyping, experimenting</t>
-  </si>
-  <si>
-    <t>Decision-making, analytical thinking, critical thinking, assess, evaluate</t>
-  </si>
-  <si>
-    <t>planning, managing, testing, process mapping, roadmap, project manage</t>
-  </si>
-  <si>
-    <t>networking, team forming, team building, connections, contacts, relationships</t>
-  </si>
-  <si>
-    <t>Negotiating, team management, persuasive, empathy, stakeholder engagement</t>
-  </si>
-  <si>
-    <t>Self-Directed, readings, supplemental activities, goal oriented, take initiative, independent, self-starter</t>
-  </si>
-  <si>
-    <t>teamwork, empathy, group management, co-founders, peers, colleagues, partners</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="5">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <sz val="12"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="4" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="4" tint="0.39997558519241921"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="4" tint="0.3999755851924192"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="4" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="4" tint="-0.499984740745262"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -334,15 +102,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -370,14 +138,74 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -677,69 +505,105 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="39.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="117.1640625" bestFit="1" customWidth="1"/>
+    <col width="39.83203125" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="117.1640625" bestFit="1" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>62</v>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Comptency</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>keyword</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>e@UBCV</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>e@UBCO</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>UBC Social Enterprise Club</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>eProjects UBC</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Enactus UBC</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Innovation UBC Hub</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Summit Leaders</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>UBC Sauder LIFT</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>UBC MBA Innovation &amp; Entrepreneurship club</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Innovation on Board</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Engineers without borders</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Startup Pitch Competition event: UBC SOAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="inlineStr">
+        <is>
+          <t>Entrepreneurial Mindset</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Entrepreneurial Mindset, entrepreneur types, traits, openness, curiosity, growth mindset, resoucefulness, resilience, grit</t>
+        </is>
       </c>
       <c r="C2" t="b">
         <v>1</v>
@@ -778,12 +642,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>63</v>
+    <row r="3">
+      <c r="A3" s="6" t="inlineStr">
+        <is>
+          <t>Opportunity Recognition</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Opportunity Recognition, opportunity identification, opportunity recognition, need finding, problem identification</t>
+        </is>
       </c>
       <c r="C3" t="b">
         <v>1</v>
@@ -822,12 +690,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
+    <row r="4">
+      <c r="A4" s="6" t="inlineStr">
+        <is>
+          <t>Market Research</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>market research, primary research, secondary research, consumer research, competitor research, customer discovery, customer validation</t>
+        </is>
       </c>
       <c r="C4" t="b">
         <v>0</v>
@@ -866,12 +738,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>64</v>
+    <row r="5">
+      <c r="A5" s="6" t="inlineStr">
+        <is>
+          <t>Product Development</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Product Development, product research, prototype, MVP, product, service development, technology research, proof of concept</t>
+        </is>
       </c>
       <c r="C5" t="b">
         <v>1</v>
@@ -910,12 +786,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
-        <v>23</v>
+    <row r="6">
+      <c r="A6" s="6" t="inlineStr">
+        <is>
+          <t>Marketing</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>marketing, channel marketing, sales, go to market strategy</t>
+        </is>
       </c>
       <c r="C6" t="b">
         <v>0</v>
@@ -954,12 +834,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" t="s">
-        <v>25</v>
+    <row r="7">
+      <c r="A7" s="6" t="inlineStr">
+        <is>
+          <t>Business Modeling</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>business model, business model canvas, go to market plan, venture forming</t>
+        </is>
       </c>
       <c r="C7" t="b">
         <v>1</v>
@@ -998,12 +882,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" t="s">
-        <v>65</v>
+    <row r="8">
+      <c r="A8" s="6" t="inlineStr">
+        <is>
+          <t>Managerial Decision Making</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Managerial Decision Making, group, project, team, management, project management, lead, decision-making</t>
+        </is>
       </c>
       <c r="C8" t="b">
         <v>1</v>
@@ -1042,12 +930,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" t="s">
-        <v>66</v>
+    <row r="9">
+      <c r="A9" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Legal </t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>legal, contracts, intellectual property, copyright, agreements, trade secrets, patents, license</t>
+        </is>
       </c>
       <c r="C9" t="b">
         <v>0</v>
@@ -1086,12 +978,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" t="s">
-        <v>30</v>
+    <row r="10">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>Financial Decision Making</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>financial, venture capital, financial modelling, investment/investing, revenue, funding</t>
+        </is>
       </c>
       <c r="C10" t="b">
         <v>0</v>
@@ -1130,12 +1026,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" t="s">
-        <v>32</v>
+    <row r="11">
+      <c r="A11" s="4" t="inlineStr">
+        <is>
+          <t>Observational skills</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>observing, questioning, seeing, sensing</t>
+        </is>
       </c>
       <c r="C11" t="b">
         <v>1</v>
@@ -1174,12 +1074,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" t="s">
-        <v>67</v>
+    <row r="12">
+      <c r="A12" s="4" t="inlineStr">
+        <is>
+          <t>Creativity skills</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>creative, associating, innovative thinking, idea generation, prototyping, experimenting</t>
+        </is>
       </c>
       <c r="C12" t="b">
         <v>1</v>
@@ -1218,12 +1122,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" t="s">
-        <v>36</v>
+    <row r="13">
+      <c r="A13" s="4" t="inlineStr">
+        <is>
+          <t>Problem solving skills</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>problem solving, problem identification, opportunity identification</t>
+        </is>
       </c>
       <c r="C13" t="b">
         <v>0</v>
@@ -1262,12 +1170,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" t="s">
-        <v>38</v>
+    <row r="14">
+      <c r="A14" s="4" t="inlineStr">
+        <is>
+          <t>Communication skills</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>presentation, present, pitch, communication, visual thinking, sketch, map, write, design, storytelling</t>
+        </is>
       </c>
       <c r="C14" t="b">
         <v>1</v>
@@ -1306,12 +1218,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" t="s">
-        <v>68</v>
+    <row r="15">
+      <c r="A15" s="4" t="inlineStr">
+        <is>
+          <t>Decision-making skills</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Decision-making, analytical thinking, critical thinking, assess, evaluate</t>
+        </is>
       </c>
       <c r="C15" t="b">
         <v>1</v>
@@ -1350,12 +1266,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" t="s">
-        <v>69</v>
+    <row r="16">
+      <c r="A16" s="4" t="inlineStr">
+        <is>
+          <t>Planning and project managing skills</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>planning, managing, testing, process mapping, roadmap, project manage</t>
+        </is>
       </c>
       <c r="C16" t="b">
         <v>1</v>
@@ -1394,12 +1314,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" t="s">
-        <v>70</v>
+    <row r="17">
+      <c r="A17" s="4" t="inlineStr">
+        <is>
+          <t>Networking skills</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>networking, team forming, team building, connections, contacts, relationships</t>
+        </is>
       </c>
       <c r="C17" t="b">
         <v>1</v>
@@ -1438,12 +1362,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" t="s">
-        <v>71</v>
+    <row r="18">
+      <c r="A18" s="4" t="inlineStr">
+        <is>
+          <t>Negotiating skills</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Negotiating, team management, persuasive, empathy, stakeholder engagement</t>
+        </is>
       </c>
       <c r="C18" t="b">
         <v>1</v>
@@ -1482,12 +1410,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" t="s">
-        <v>48</v>
+    <row r="19">
+      <c r="A19" s="5" t="inlineStr">
+        <is>
+          <t>Self-Aware</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>risk-tolerant, open, take initiative, enterprising, committed, traits</t>
+        </is>
       </c>
       <c r="C19" t="b">
         <v>1</v>
@@ -1526,12 +1458,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" t="s">
-        <v>50</v>
+    <row r="20">
+      <c r="A20" s="5" t="inlineStr">
+        <is>
+          <t>Enterprising Traits</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>curiosity, self-motivated, experimental, confident, competitive, pro-active</t>
+        </is>
       </c>
       <c r="C20" t="b">
         <v>1</v>
@@ -1570,12 +1506,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B21" t="s">
-        <v>72</v>
+    <row r="21">
+      <c r="A21" s="5" t="inlineStr">
+        <is>
+          <t>Self-Directed</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Self-Directed, readings, supplemental activities, goal oriented, take initiative, independent, self-starter</t>
+        </is>
       </c>
       <c r="C21" t="b">
         <v>1</v>
@@ -1614,12 +1554,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" t="s">
-        <v>73</v>
+    <row r="22">
+      <c r="A22" s="5" t="inlineStr">
+        <is>
+          <t>Teamwork</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>teamwork, empathy, group management, co-founders, peers, colleagues, partners</t>
+        </is>
       </c>
       <c r="C22" t="b">
         <v>1</v>
@@ -1658,12 +1602,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B23" t="s">
-        <v>56</v>
+    <row r="23">
+      <c r="A23" s="5" t="inlineStr">
+        <is>
+          <t>Uncertainty Management</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>uncertainty, ambiguity, navigation, unfamiliar, volitility, risk, complexity</t>
+        </is>
       </c>
       <c r="C23" t="b">
         <v>1</v>
@@ -1704,165 +1652,231 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:N1048576">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="true">
+    <cfRule type="containsText" priority="1" operator="containsText" dxfId="1" text="true">
       <formula>NOT(ISERROR(SEARCH("true",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="false">
+    <cfRule type="containsText" priority="2" operator="containsText" dxfId="0" text="false">
       <formula>NOT(ISERROR(SEARCH("false",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C1" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D1" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C1" r:id="rId1"/>
+    <hyperlink ref="D1" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="A1" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>57</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>e@UBCV</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>e@UBCO</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>UBC Social Enterprise Club</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>eProjects UBC</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Enactus UBC</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Innovation UBC Hub</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Summit Leaders</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>UBC Sauder LIFT</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>UBC MBA Innovation &amp; Entrepreneurship club</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Innovation on Board</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Engineers without borders</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Startup Pitch Competition event: UBC SOAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>LaunchWeek</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="A1" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:N23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
+    <row r="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>Comptency</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>keyword</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>e@UBCV</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>e@UBCO</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>UBC Social Enterprise Club</t>
+        </is>
+      </c>
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>eProjects UBC</t>
+        </is>
+      </c>
+      <c r="G1" s="3" t="inlineStr">
+        <is>
+          <t>Enactus UBC</t>
+        </is>
+      </c>
+      <c r="H1" s="3" t="inlineStr">
+        <is>
+          <t>Innovation UBC Hub</t>
+        </is>
+      </c>
+      <c r="I1" s="3" t="inlineStr">
+        <is>
+          <t>Summit Leaders</t>
+        </is>
+      </c>
+      <c r="J1" s="3" t="inlineStr">
+        <is>
+          <t>UBC Sauder LIFT</t>
+        </is>
+      </c>
+      <c r="K1" s="3" t="inlineStr">
+        <is>
+          <t>UBC MBA Innovation &amp; Entrepreneurship club</t>
+        </is>
+      </c>
+      <c r="L1" s="3" t="inlineStr">
+        <is>
+          <t>Innovation on Board</t>
+        </is>
+      </c>
+      <c r="M1" s="3" t="inlineStr">
+        <is>
+          <t>Engineers without borders</t>
+        </is>
+      </c>
+      <c r="N1" s="3" t="inlineStr">
+        <is>
+          <t>Startup Pitch Competition event: UBC SOAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Entrepreneurial Mindset</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>entrepreneur types, traits, openness, curiosity, growth mindset, resoucefulness, resilience, grit</t>
+        </is>
       </c>
       <c r="C2" t="b">
         <v>1</v>
@@ -1901,12 +1915,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Opportunity Recognition</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>opportunity identification, opportunity recognition, need finding, problem identification</t>
+        </is>
       </c>
       <c r="C3" t="b">
         <v>1</v>
@@ -1945,12 +1963,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>58</v>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Market Research</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>market research, primary research, secondary research, consumer research, competitor research</t>
+        </is>
       </c>
       <c r="C4" t="b">
         <v>0</v>
@@ -1989,12 +2011,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Product Development</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>product research, prototype, MVP, product, service development, technology research, proof of concept</t>
+        </is>
       </c>
       <c r="C5" t="b">
         <v>1</v>
@@ -2033,12 +2059,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
-        <v>59</v>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Marketing</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>marketing, channel marketing, sales, go to market strategy, customer discovery, customer validation</t>
+        </is>
       </c>
       <c r="C6" t="b">
         <v>0</v>
@@ -2077,12 +2107,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" t="s">
-        <v>25</v>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Business Modeling</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>business model, business model canvas, go to market plan, venture forming</t>
+        </is>
       </c>
       <c r="C7" t="b">
         <v>1</v>
@@ -2121,12 +2155,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" t="s">
-        <v>27</v>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Managerial Decision Making</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>group, project, team, management, project management, lead, decision-making</t>
+        </is>
       </c>
       <c r="C8" t="b">
         <v>1</v>
@@ -2165,12 +2203,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" t="s">
-        <v>60</v>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Legal </t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>legal matters, contracts, intellectual property, copyright, agreements, trade secrets</t>
+        </is>
       </c>
       <c r="C9" t="b">
         <v>0</v>
@@ -2209,12 +2251,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" t="s">
-        <v>30</v>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Financial Decision Making</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>financial, venture capital, financial modelling, investment/investing, revenue, funding</t>
+        </is>
       </c>
       <c r="C10" t="b">
         <v>0</v>
@@ -2253,12 +2299,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" t="s">
-        <v>32</v>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Observational skills</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>observing, questioning, seeing, sensing</t>
+        </is>
       </c>
       <c r="C11" t="b">
         <v>1</v>
@@ -2297,12 +2347,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" t="s">
-        <v>34</v>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Creativity skills</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>associating, creative thinking, innovative thinking, idea generation, prototyping, experimenting</t>
+        </is>
       </c>
       <c r="C12" t="b">
         <v>1</v>
@@ -2341,12 +2395,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" t="s">
-        <v>36</v>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Problem solving skills</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>problem solving, problem identification, opportunity identification</t>
+        </is>
       </c>
       <c r="C13" t="b">
         <v>0</v>
@@ -2385,12 +2443,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" t="s">
-        <v>38</v>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Communication skills</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>presentation, present, pitch, communication, visual thinking, sketch, map, write, design, storytelling</t>
+        </is>
       </c>
       <c r="C14" t="b">
         <v>1</v>
@@ -2429,12 +2491,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" t="s">
-        <v>40</v>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Decision-making skills</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>analytical thinking, critical thinking, assess, evaluate</t>
+        </is>
       </c>
       <c r="C15" t="b">
         <v>1</v>
@@ -2473,12 +2539,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" t="s">
-        <v>42</v>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Planning and project managing skills</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>testing, process mapping, roadmap, project manage</t>
+        </is>
       </c>
       <c r="C16" t="b">
         <v>1</v>
@@ -2517,12 +2587,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" t="s">
-        <v>44</v>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Networking skills</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>team forming, team building, connections, contacts, relationships</t>
+        </is>
       </c>
       <c r="C17" t="b">
         <v>1</v>
@@ -2561,12 +2635,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" t="s">
-        <v>46</v>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Negotiating skills</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>team management, persuasive, empathy, stakeholder engagement</t>
+        </is>
       </c>
       <c r="C18" t="b">
         <v>1</v>
@@ -2605,12 +2683,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" t="s">
-        <v>48</v>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Self-Aware</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>risk-tolerant, open, take initiative, enterprising, committed, traits</t>
+        </is>
       </c>
       <c r="C19" t="b">
         <v>1</v>
@@ -2649,12 +2731,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>61</v>
-      </c>
-      <c r="B20" t="s">
-        <v>50</v>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Enterprising Mindset</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>curiosity, self-motivated, experimental, confident, competitive, pro-active</t>
+        </is>
       </c>
       <c r="C20" t="b">
         <v>1</v>
@@ -2693,12 +2779,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>51</v>
-      </c>
-      <c r="B21" t="s">
-        <v>52</v>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Self-Directed</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>readings, supplemental activities, goal oriented, take initiative, independent, self-starter</t>
+        </is>
       </c>
       <c r="C21" t="b">
         <v>1</v>
@@ -2737,12 +2827,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" t="s">
-        <v>54</v>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Teamwork</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>networking, empathy, group management, co-founders, peers, colleagues, partners</t>
+        </is>
       </c>
       <c r="C22" t="b">
         <v>1</v>
@@ -2781,12 +2875,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>55</v>
-      </c>
-      <c r="B23" t="s">
-        <v>56</v>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Uncertainty Management</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>uncertainty, ambiguity, navigation, unfamiliar, volitility, risk, complexity</t>
+        </is>
       </c>
       <c r="C23" t="b">
         <v>1</v>

</xml_diff>